<commit_message>
Monthly output fixed for averaging
</commit_message>
<xml_diff>
--- a/TaskWorksheets/Clinac_MonthlyOutput.xlsx
+++ b/TaskWorksheets/Clinac_MonthlyOutput.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17571"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcardan\OneDrive\Cardan.Code\Git\Autodrive\TaskWorksheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rex\OneDrive\Cardan.Code\Git\Autodrive\TaskWorksheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="19200" windowHeight="8670" tabRatio="494" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="19200" windowHeight="8673" tabRatio="494" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Autodrive" sheetId="12" r:id="rId1"/>
@@ -245,7 +245,7 @@
     <definedName name="T">MEASURE!$J$4</definedName>
     <definedName name="test">CurrentSelections!$L$32:$L$34</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -3565,27 +3565,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="18" borderId="103" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="66" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="67" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="8" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="71" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="72" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="68" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -3593,6 +3572,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="65" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="21" borderId="66" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3603,6 +3585,15 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="21" borderId="29" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="66" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="67" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="68" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="10" borderId="16" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -3630,6 +3621,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="70" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="8" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="71" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="72" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="7" borderId="24" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3661,6 +3661,30 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="62" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="29" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="79" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="67" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="79" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="67" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="79" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="80" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="27" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="11" borderId="0" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3685,9 +3709,6 @@
     <xf numFmtId="0" fontId="19" fillId="7" borderId="84" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="29" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="7" borderId="85" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3700,38 +3721,14 @@
     <xf numFmtId="0" fontId="6" fillId="15" borderId="79" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="79" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="67" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="79" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="67" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="79" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="80" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="27" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="86" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="28" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="15" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="87" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3742,14 +3739,11 @@
     <xf numFmtId="0" fontId="19" fillId="7" borderId="89" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="90" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="91" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="18" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="15" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="27" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3757,8 +3751,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="91" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="18" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="90" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="27" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="47" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="2" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3797,9 +3800,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="99" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="47" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="77" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4475,7 +4475,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4521,13 +4521,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>30</xdr:row>
-          <xdr:rowOff>200025</xdr:rowOff>
+          <xdr:rowOff>198967</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>971550</xdr:colOff>
+          <xdr:colOff>973667</xdr:colOff>
           <xdr:row>34</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>173567</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4559,7 +4559,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="27432" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="54864" tIns="41148" rIns="54864" bIns="41148" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -4593,9 +4593,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>676275</xdr:colOff>
+          <xdr:colOff>677333</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>219075</xdr:rowOff>
+          <xdr:rowOff>220133</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4627,7 +4627,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="27432" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="54864" tIns="41148" rIns="54864" bIns="41148" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -4661,7 +4661,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>962025</xdr:colOff>
+          <xdr:colOff>960967</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -4695,7 +4695,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="27432" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="54864" tIns="41148" rIns="54864" bIns="41148" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -5269,19 +5269,19 @@
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.609375" defaultRowHeight="14" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="8.625" style="114" customWidth="1"/>
-    <col min="3" max="3" width="10.375" style="114" customWidth="1"/>
-    <col min="4" max="8" width="8.625" style="114" customWidth="1"/>
+    <col min="1" max="2" width="8.609375" style="114" customWidth="1"/>
+    <col min="3" max="3" width="10.38671875" style="114" customWidth="1"/>
+    <col min="4" max="8" width="8.609375" style="114" customWidth="1"/>
     <col min="9" max="9" width="12" style="114" customWidth="1"/>
     <col min="10" max="10" width="15" style="114" customWidth="1"/>
-    <col min="11" max="11" width="17.125" style="114" customWidth="1"/>
-    <col min="12" max="12" width="8.625" style="114" customWidth="1"/>
-    <col min="13" max="16384" width="8.625" style="114"/>
+    <col min="11" max="11" width="17.109375" style="114" customWidth="1"/>
+    <col min="12" max="12" width="8.609375" style="114" customWidth="1"/>
+    <col min="13" max="16384" width="8.609375" style="114"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A1" s="114" t="s">
         <v>108</v>
       </c>
@@ -5325,7 +5325,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A2" s="115" t="s">
         <v>122</v>
       </c>
@@ -5361,7 +5361,7 @@
       <c r="M2" s="115"/>
       <c r="N2" s="115"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A3" s="115" t="s">
         <v>124</v>
       </c>
@@ -5397,7 +5397,7 @@
       <c r="M3" s="115"/>
       <c r="N3" s="115"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A4" s="115" t="s">
         <v>122</v>
       </c>
@@ -5433,7 +5433,7 @@
       <c r="M4" s="115"/>
       <c r="N4" s="115"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A5" s="115" t="s">
         <v>124</v>
       </c>
@@ -5469,7 +5469,7 @@
       <c r="M5" s="115"/>
       <c r="N5" s="115"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A6" s="115" t="s">
         <v>9</v>
       </c>
@@ -5499,7 +5499,7 @@
       <c r="M6" s="115"/>
       <c r="N6" s="115"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A7" s="115" t="s">
         <v>9</v>
       </c>
@@ -5529,7 +5529,7 @@
       <c r="M7" s="115"/>
       <c r="N7" s="115"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A8" s="115" t="s">
         <v>10</v>
       </c>
@@ -5559,7 +5559,7 @@
       <c r="M8" s="115"/>
       <c r="N8" s="115"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A9" s="115" t="s">
         <v>10</v>
       </c>
@@ -5589,7 +5589,7 @@
       <c r="M9" s="115"/>
       <c r="N9" s="115"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A10" s="115" t="s">
         <v>11</v>
       </c>
@@ -5619,7 +5619,7 @@
       <c r="M10" s="115"/>
       <c r="N10" s="115"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A11" s="115" t="s">
         <v>11</v>
       </c>
@@ -5649,7 +5649,7 @@
       <c r="M11" s="115"/>
       <c r="N11" s="115"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A12" s="115" t="s">
         <v>12</v>
       </c>
@@ -5679,7 +5679,7 @@
       <c r="M12" s="115"/>
       <c r="N12" s="115"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A13" s="115" t="s">
         <v>12</v>
       </c>
@@ -5709,7 +5709,7 @@
       <c r="M13" s="115"/>
       <c r="N13" s="115"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A14" s="115" t="s">
         <v>13</v>
       </c>
@@ -5739,7 +5739,7 @@
       <c r="M14" s="115"/>
       <c r="N14" s="115"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A15" s="115" t="s">
         <v>13</v>
       </c>
@@ -5783,57 +5783,57 @@
   </sheetPr>
   <dimension ref="B1:L46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="90" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="4.375" customWidth="1"/>
+    <col min="1" max="1" width="4.38671875" customWidth="1"/>
     <col min="2" max="2" width="11.5" customWidth="1"/>
-    <col min="3" max="3" width="8.125" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="5" max="5" width="10.375" customWidth="1"/>
-    <col min="6" max="6" width="25.375" customWidth="1"/>
-    <col min="7" max="7" width="15.625" customWidth="1"/>
-    <col min="8" max="9" width="18.375" customWidth="1"/>
+    <col min="5" max="5" width="10.38671875" customWidth="1"/>
+    <col min="6" max="6" width="25.38671875" customWidth="1"/>
+    <col min="7" max="7" width="15.609375" customWidth="1"/>
+    <col min="8" max="9" width="18.38671875" customWidth="1"/>
     <col min="10" max="10" width="24" customWidth="1"/>
-    <col min="11" max="11" width="12.875" customWidth="1"/>
-    <col min="12" max="12" width="4.625" customWidth="1"/>
-    <col min="15" max="15" width="37.375" customWidth="1"/>
+    <col min="11" max="11" width="12.88671875" customWidth="1"/>
+    <col min="12" max="12" width="4.609375" customWidth="1"/>
+    <col min="15" max="15" width="37.38671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B1" s="137" t="s">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B1" s="130" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="137"/>
-      <c r="D1" s="137"/>
-      <c r="E1" s="137"/>
-      <c r="F1" s="137"/>
-      <c r="G1" s="137"/>
-      <c r="H1" s="138" t="s">
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="130"/>
+      <c r="H1" s="131" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="138"/>
-      <c r="J1" s="138"/>
-      <c r="K1" s="138"/>
+      <c r="I1" s="131"/>
+      <c r="J1" s="131"/>
+      <c r="K1" s="131"/>
       <c r="L1" s="39"/>
     </row>
-    <row r="2" spans="2:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="137"/>
-      <c r="C2" s="137"/>
-      <c r="D2" s="137"/>
-      <c r="E2" s="137"/>
-      <c r="F2" s="137"/>
-      <c r="G2" s="137"/>
-      <c r="H2" s="138"/>
-      <c r="I2" s="138"/>
-      <c r="J2" s="138"/>
-      <c r="K2" s="138"/>
+    <row r="2" spans="2:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="130"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
+      <c r="F2" s="130"/>
+      <c r="G2" s="130"/>
+      <c r="H2" s="131"/>
+      <c r="I2" s="131"/>
+      <c r="J2" s="131"/>
+      <c r="K2" s="131"/>
       <c r="L2" s="39"/>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B3" s="36"/>
       <c r="C3" s="36"/>
       <c r="D3" s="36"/>
@@ -5841,10 +5841,10 @@
       <c r="F3" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="145" t="s">
+      <c r="G3" s="142" t="s">
         <v>58</v>
       </c>
-      <c r="H3" s="146"/>
+      <c r="H3" s="143"/>
       <c r="I3" s="38" t="s">
         <v>63</v>
       </c>
@@ -5853,7 +5853,7 @@
       </c>
       <c r="L3" s="39"/>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
       <c r="D4" s="36"/>
@@ -5861,8 +5861,8 @@
       <c r="F4" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="143"/>
-      <c r="H4" s="144"/>
+      <c r="G4" s="140"/>
+      <c r="H4" s="141"/>
       <c r="I4" s="37" t="s">
         <v>18</v>
       </c>
@@ -5872,19 +5872,19 @@
       </c>
       <c r="L4" s="39"/>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B5" s="36"/>
       <c r="C5" s="36"/>
       <c r="D5" s="36"/>
-      <c r="E5" s="150" t="str">
+      <c r="E5" s="147" t="str">
         <f>"Ion Chamber (Cal: "&amp;TEXT(Current_Chamber_CalDate,"mm/dd/yyyy")&amp;")"</f>
         <v>Ion Chamber (Cal: 11/09/2016)</v>
       </c>
-      <c r="F5" s="151"/>
-      <c r="G5" s="145" t="s">
+      <c r="F5" s="148"/>
+      <c r="G5" s="142" t="s">
         <v>65</v>
       </c>
-      <c r="H5" s="146"/>
+      <c r="H5" s="143"/>
       <c r="I5" s="37" t="s">
         <v>19</v>
       </c>
@@ -5894,19 +5894,19 @@
       </c>
       <c r="L5" s="39"/>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B6" s="36"/>
       <c r="C6" s="36"/>
       <c r="D6" s="36"/>
-      <c r="E6" s="150" t="str">
+      <c r="E6" s="147" t="str">
         <f>"Electrometer (Cal: "&amp;TEXT(Current_Electrometer_CalDate,"mm/dd/yyyy")&amp;")"</f>
         <v>Electrometer (Cal: 11/05/2015)</v>
       </c>
-      <c r="F6" s="151"/>
-      <c r="G6" s="145" t="s">
+      <c r="F6" s="148"/>
+      <c r="G6" s="142" t="s">
         <v>104</v>
       </c>
-      <c r="H6" s="146"/>
+      <c r="H6" s="143"/>
       <c r="I6" s="38" t="s">
         <v>25</v>
       </c>
@@ -5917,7 +5917,7 @@
       <c r="K6" s="36"/>
       <c r="L6" s="39"/>
     </row>
-    <row r="7" spans="2:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="39"/>
       <c r="C7" s="39"/>
       <c r="D7" s="39"/>
@@ -5930,7 +5930,7 @@
       <c r="K7" s="39"/>
       <c r="L7" s="39"/>
     </row>
-    <row r="8" spans="2:12" ht="6.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" ht="6.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="39"/>
       <c r="C8" s="39"/>
       <c r="D8" s="39"/>
@@ -5943,36 +5943,36 @@
       <c r="K8" s="39"/>
       <c r="L8" s="39"/>
     </row>
-    <row r="9" spans="2:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="147" t="s">
+    <row r="9" spans="2:12" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B9" s="144" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="148"/>
-      <c r="D9" s="148"/>
-      <c r="E9" s="148"/>
-      <c r="F9" s="148"/>
-      <c r="G9" s="148"/>
-      <c r="H9" s="148"/>
-      <c r="I9" s="148"/>
-      <c r="J9" s="148"/>
-      <c r="K9" s="149"/>
-    </row>
-    <row r="10" spans="2:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="130" t="str">
+      <c r="C9" s="145"/>
+      <c r="D9" s="145"/>
+      <c r="E9" s="145"/>
+      <c r="F9" s="145"/>
+      <c r="G9" s="145"/>
+      <c r="H9" s="145"/>
+      <c r="I9" s="145"/>
+      <c r="J9" s="145"/>
+      <c r="K9" s="146"/>
+    </row>
+    <row r="10" spans="2:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B10" s="137" t="str">
         <f>INDEX(Machines!A5:AF20,MATCH(MEASURE!H1,Machines,0),2)&amp;"X"</f>
         <v>6X</v>
       </c>
-      <c r="C10" s="131"/>
-      <c r="D10" s="131"/>
-      <c r="E10" s="131"/>
-      <c r="F10" s="131"/>
-      <c r="G10" s="131"/>
-      <c r="H10" s="131"/>
-      <c r="I10" s="131"/>
-      <c r="J10" s="131"/>
-      <c r="K10" s="136"/>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C10" s="138"/>
+      <c r="D10" s="138"/>
+      <c r="E10" s="138"/>
+      <c r="F10" s="138"/>
+      <c r="G10" s="138"/>
+      <c r="H10" s="138"/>
+      <c r="I10" s="138"/>
+      <c r="J10" s="138"/>
+      <c r="K10" s="139"/>
+    </row>
+    <row r="11" spans="2:12" ht="15" x14ac:dyDescent="0.45">
       <c r="B11" s="21"/>
       <c r="C11" s="133" t="s">
         <v>60</v>
@@ -5996,7 +5996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:12" ht="15" x14ac:dyDescent="0.4">
       <c r="B12" s="14" t="s">
         <v>2</v>
       </c>
@@ -6025,7 +6025,7 @@
       </c>
       <c r="K12" s="117"/>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B13" s="14">
         <f>Current_dmax_LowX</f>
         <v>1.6</v>
@@ -6034,13 +6034,13 @@
         <f>Autodrive!L4*-100000000</f>
         <v>0</v>
       </c>
-      <c r="D13" s="3">
-        <f>Autodrive!M4*-100000000</f>
+      <c r="D13" s="3" t="str">
+        <f>IF(ABS(Autodrive!M4*-100000000)&gt;0,ABS(Autodrive!M4*-100000000)&gt;0,"")</f>
+        <v/>
+      </c>
+      <c r="E13" s="23">
+        <f>IFERROR(AVERAGE(C13:D13),"")</f>
         <v>0</v>
-      </c>
-      <c r="E13" s="23" t="str">
-        <f>IFERROR(AVERAGEIF(C13:D13,"&lt;&gt;0"),"")</f>
-        <v/>
       </c>
       <c r="F13" s="23" t="str">
         <f>IFERROR(E13*Current_Ppol_LowX*Current_Pion_LowX*Current_Pelec*CTP,"")</f>
@@ -6064,7 +6064,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:12" ht="14.35" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B14" s="14">
         <v>10</v>
       </c>
@@ -6072,13 +6072,13 @@
         <f>Autodrive!L2*-100000000</f>
         <v>0</v>
       </c>
-      <c r="D14" s="19">
-        <f>Autodrive!M2*-100000000</f>
+      <c r="D14" s="19" t="str">
+        <f>IF(ABS(Autodrive!M2*-100000000)&gt;0,ABS(Autodrive!M2*-100000000)&gt;0,"")</f>
+        <v/>
+      </c>
+      <c r="E14" s="23">
+        <f>IFERROR(AVERAGE(C14:D14),"")</f>
         <v>0</v>
-      </c>
-      <c r="E14" s="23" t="str">
-        <f>IFERROR(AVERAGEIF(C14:D14,"&lt;&gt;0"),"")</f>
-        <v/>
       </c>
       <c r="F14" s="23" t="str">
         <f>IFERROR(E14*Current_Ppol_LowX*Current_Pelec*Current_Pion_LowX*CTP,"")</f>
@@ -6105,22 +6105,22 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="2:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="134" t="str">
+    <row r="15" spans="2:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B15" s="150" t="str">
         <f>INDEX(Machines!A5:AF20,MATCH(MEASURE!H1,Machines,0),3)&amp;"X"</f>
         <v>15X</v>
       </c>
-      <c r="C15" s="135"/>
-      <c r="D15" s="135"/>
-      <c r="E15" s="135"/>
-      <c r="F15" s="135"/>
-      <c r="G15" s="135"/>
-      <c r="H15" s="135"/>
-      <c r="I15" s="135"/>
-      <c r="J15" s="135"/>
-      <c r="K15" s="132"/>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C15" s="151"/>
+      <c r="D15" s="151"/>
+      <c r="E15" s="151"/>
+      <c r="F15" s="151"/>
+      <c r="G15" s="151"/>
+      <c r="H15" s="151"/>
+      <c r="I15" s="151"/>
+      <c r="J15" s="151"/>
+      <c r="K15" s="149"/>
+    </row>
+    <row r="16" spans="2:12" ht="15" x14ac:dyDescent="0.45">
       <c r="B16" s="21"/>
       <c r="C16" s="133" t="s">
         <v>60</v>
@@ -6130,10 +6130,10 @@
       <c r="F16" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="G16" s="139" t="s">
+      <c r="G16" s="132" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="139"/>
+      <c r="H16" s="132"/>
       <c r="I16" s="22" t="s">
         <v>24</v>
       </c>
@@ -6144,7 +6144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" ht="15" x14ac:dyDescent="0.4">
       <c r="B17" s="14" t="s">
         <v>2</v>
       </c>
@@ -6173,7 +6173,7 @@
       </c>
       <c r="K17" s="119"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B18" s="14">
         <f>Current_dmax_HighX</f>
         <v>2.7</v>
@@ -6182,13 +6182,13 @@
         <f>Autodrive!L5*-100000000</f>
         <v>0</v>
       </c>
-      <c r="D18" s="3">
-        <f>Autodrive!M5*-100000000</f>
+      <c r="D18" s="3" t="str">
+        <f>IF(ABS(Autodrive!M5*-100000000)&gt;0,ABS(Autodrive!M5*-100000000)&gt;0,"")</f>
+        <v/>
+      </c>
+      <c r="E18" s="23">
+        <f>IFERROR(AVERAGE(C18:D18),"")</f>
         <v>0</v>
-      </c>
-      <c r="E18" s="23" t="str">
-        <f>IFERROR(AVERAGEIF(C18:D18,"&lt;&gt;0"),"")</f>
-        <v/>
       </c>
       <c r="F18" s="4" t="str">
         <f>IFERROR(E18*Current_Ppol_HighX*Current_Pion_HighX*Current_Pelec*CTP,"")</f>
@@ -6212,7 +6212,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:11" ht="14.35" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="14">
         <v>10</v>
       </c>
@@ -6220,13 +6220,13 @@
         <f>Autodrive!L3*-100000000</f>
         <v>0</v>
       </c>
-      <c r="D19" s="19">
-        <f>Autodrive!M3*-100000000</f>
+      <c r="D19" s="19" t="str">
+        <f>IF(ABS(Autodrive!M3*-100000000)&gt;0,ABS(Autodrive!M3*-100000000)&gt;0,"")</f>
+        <v/>
+      </c>
+      <c r="E19" s="23">
+        <f>IFERROR(AVERAGE(C19:D19),"")</f>
         <v>0</v>
-      </c>
-      <c r="E19" s="23" t="str">
-        <f>IFERROR(AVERAGEIF(C19:D19,"&lt;&gt;0"),"")</f>
-        <v/>
       </c>
       <c r="F19" s="23" t="str">
         <f>IFERROR(E19*Current_Ppol_HighX*Current_Pion_HighX*Current_Pelec*CTP,"")</f>
@@ -6253,37 +6253,37 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="140" t="s">
+    <row r="20" spans="2:11" ht="6" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="21" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B21" s="134" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="141"/>
-      <c r="D21" s="141"/>
-      <c r="E21" s="141"/>
-      <c r="F21" s="141"/>
-      <c r="G21" s="141"/>
-      <c r="H21" s="141"/>
-      <c r="I21" s="141"/>
-      <c r="J21" s="141"/>
-      <c r="K21" s="142"/>
-    </row>
-    <row r="22" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="130" t="str">
+      <c r="C21" s="135"/>
+      <c r="D21" s="135"/>
+      <c r="E21" s="135"/>
+      <c r="F21" s="135"/>
+      <c r="G21" s="135"/>
+      <c r="H21" s="135"/>
+      <c r="I21" s="135"/>
+      <c r="J21" s="135"/>
+      <c r="K21" s="136"/>
+    </row>
+    <row r="22" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B22" s="137" t="str">
         <f>INDEX(Machines!A5:AF20,MATCH(MEASURE!H1,Machines,0),4)&amp;"E"</f>
         <v>6E</v>
       </c>
-      <c r="C22" s="131"/>
-      <c r="D22" s="131"/>
-      <c r="E22" s="131"/>
-      <c r="F22" s="131"/>
-      <c r="G22" s="131"/>
-      <c r="H22" s="131"/>
-      <c r="I22" s="131"/>
-      <c r="J22" s="131"/>
-      <c r="K22" s="136"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C22" s="138"/>
+      <c r="D22" s="138"/>
+      <c r="E22" s="138"/>
+      <c r="F22" s="138"/>
+      <c r="G22" s="138"/>
+      <c r="H22" s="138"/>
+      <c r="I22" s="138"/>
+      <c r="J22" s="138"/>
+      <c r="K22" s="139"/>
+    </row>
+    <row r="23" spans="2:11" ht="15" x14ac:dyDescent="0.45">
       <c r="B23" s="21"/>
       <c r="C23" s="133" t="s">
         <v>60</v>
@@ -6305,7 +6305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:11" ht="15" x14ac:dyDescent="0.4">
       <c r="B24" s="14" t="s">
         <v>2</v>
       </c>
@@ -6333,7 +6333,7 @@
       </c>
       <c r="K24" s="120"/>
     </row>
-    <row r="25" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:11" ht="14.35" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B25" s="51" t="str">
         <f>TEXT(Current_dref_E1+0.5*Current_rcav,"0.00")</f>
         <v>1.48</v>
@@ -6342,13 +6342,13 @@
         <f>Autodrive!L6*-100000000</f>
         <v>0</v>
       </c>
-      <c r="D25" s="3">
-        <f>Autodrive!M6*-100000000</f>
+      <c r="D25" s="3" t="str">
+        <f>IF(ABS(Autodrive!M6*-100000000)&gt;0,ABS(Autodrive!M6*-100000000)&gt;0,"")</f>
+        <v/>
+      </c>
+      <c r="E25" s="23">
+        <f>IFERROR(AVERAGE(C25:D25),"")</f>
         <v>0</v>
-      </c>
-      <c r="E25" s="23" t="str">
-        <f>IFERROR(AVERAGEIF(C25:D25,"&lt;&gt;0"),"")</f>
-        <v/>
       </c>
       <c r="F25" s="4" t="str">
         <f>IFERROR(E25*Current_Ppol_E1*Current_Pion_E1*Current_Pelec*CTP,"")</f>
@@ -6375,7 +6375,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B26" s="51" t="str">
         <f>TEXT(Current_R80_E1+0.5*Current_rcav,"0.00")</f>
         <v>2.15</v>
@@ -6384,13 +6384,13 @@
         <f>Autodrive!L7*-100000000</f>
         <v>0</v>
       </c>
-      <c r="D26" s="3">
-        <f>Autodrive!M7*-100000000</f>
+      <c r="D26" s="3" t="str">
+        <f>IF(ABS(Autodrive!M7*-100000000)&gt;0,ABS(Autodrive!M7*-100000000)&gt;0,"")</f>
+        <v/>
+      </c>
+      <c r="E26" s="23">
+        <f>IFERROR(AVERAGE(C26:D26),"")</f>
         <v>0</v>
-      </c>
-      <c r="E26" s="23" t="str">
-        <f>IFERROR(AVERAGEIF(C26:D26,"&lt;&gt;0"),"")</f>
-        <v/>
       </c>
       <c r="F26" s="4" t="str">
         <f>IFERROR(E26*Current_Ppol_E1*Current_Pion_E1*Current_Pelec*CTP,"")</f>
@@ -6411,25 +6411,25 @@
       </c>
       <c r="K26" s="95" t="str">
         <f>IF(ISNUMBER(E26),IFERROR(IF(AND(I26&gt;Current_LowETol_E1,I26&lt;Current_HighETol_E1),"PASSED","ENERGY FAIL"),""),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="130" t="str">
+        <v>ENERGY FAIL</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B27" s="137" t="str">
         <f>INDEX(Machines!A5:AF20,MATCH(MEASURE!H1,Machines,0),5)&amp;"E"</f>
         <v>9E</v>
       </c>
-      <c r="C27" s="131"/>
-      <c r="D27" s="131"/>
-      <c r="E27" s="131"/>
-      <c r="F27" s="131"/>
-      <c r="G27" s="131"/>
-      <c r="H27" s="131"/>
-      <c r="I27" s="131"/>
-      <c r="J27" s="131"/>
-      <c r="K27" s="132"/>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C27" s="138"/>
+      <c r="D27" s="138"/>
+      <c r="E27" s="138"/>
+      <c r="F27" s="138"/>
+      <c r="G27" s="138"/>
+      <c r="H27" s="138"/>
+      <c r="I27" s="138"/>
+      <c r="J27" s="138"/>
+      <c r="K27" s="149"/>
+    </row>
+    <row r="28" spans="2:11" ht="15" x14ac:dyDescent="0.45">
       <c r="B28" s="21"/>
       <c r="C28" s="133" t="s">
         <v>60</v>
@@ -6451,7 +6451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:11" ht="15" x14ac:dyDescent="0.4">
       <c r="B29" s="14" t="s">
         <v>2</v>
       </c>
@@ -6479,7 +6479,7 @@
       </c>
       <c r="K29" s="122"/>
     </row>
-    <row r="30" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:11" ht="14.35" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B30" s="51" t="str">
         <f>TEXT(Current_dref_E2+0.5*Current_rcav,"0.00")</f>
         <v>2.21</v>
@@ -6488,13 +6488,13 @@
         <f>Autodrive!L8*-100000000</f>
         <v>0</v>
       </c>
-      <c r="D30" s="3">
-        <f>Autodrive!M8*-100000000</f>
+      <c r="D30" s="3" t="str">
+        <f>IF(ABS(Autodrive!M8*-100000000)&gt;0,ABS(Autodrive!M8*-100000000)&gt;0,"")</f>
+        <v/>
+      </c>
+      <c r="E30" s="23">
+        <f>IFERROR(AVERAGE(C30:D30),"")</f>
         <v>0</v>
-      </c>
-      <c r="E30" s="23" t="str">
-        <f>IFERROR(AVERAGEIF(C30:D30,"&lt;&gt;0"),"")</f>
-        <v/>
       </c>
       <c r="F30" s="4" t="str">
         <f>IFERROR(E30*Current_Ppol_E2*Current_Pion_E2*Current_Pelec*CTP,"")</f>
@@ -6521,7 +6521,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B31" s="51" t="str">
         <f>TEXT(Current_R80_E2+0.5*Current_rcav,"0.00")</f>
         <v>3.15</v>
@@ -6530,13 +6530,13 @@
         <f>Autodrive!L9*-100000000</f>
         <v>0</v>
       </c>
-      <c r="D31" s="3">
-        <f>Autodrive!M9*-100000000</f>
+      <c r="D31" s="3" t="str">
+        <f>IF(ABS(Autodrive!M9*-100000000)&gt;0,ABS(Autodrive!M9*-100000000)&gt;0,"")</f>
+        <v/>
+      </c>
+      <c r="E31" s="23">
+        <f>IFERROR(AVERAGE(C31:D31),"")</f>
         <v>0</v>
-      </c>
-      <c r="E31" s="23" t="str">
-        <f>IFERROR(AVERAGEIF(C31:D31,"&lt;&gt;0"),"")</f>
-        <v/>
       </c>
       <c r="F31" s="4" t="str">
         <f>IFERROR(E31*Current_Ppol_E2*Current_Pion_E2*Current_Pelec*CTP,"")</f>
@@ -6557,25 +6557,25 @@
       </c>
       <c r="K31" s="95" t="str">
         <f>IF(ISNUMBER(E31),IFERROR(IF(AND(I31&gt;Current_LowETol_E1,I31&lt;Current_HighETol_E1),"PASSED","ENERGY FAIL"),""),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="130" t="str">
+        <v>ENERGY FAIL</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B32" s="137" t="str">
         <f>INDEX(Machines!A5:AF20,MATCH(MEASURE!H1,Machines,0),6)&amp;"E"</f>
         <v>12E</v>
       </c>
-      <c r="C32" s="131"/>
-      <c r="D32" s="131"/>
-      <c r="E32" s="131"/>
-      <c r="F32" s="131"/>
-      <c r="G32" s="131"/>
-      <c r="H32" s="131"/>
-      <c r="I32" s="131"/>
-      <c r="J32" s="131"/>
-      <c r="K32" s="132"/>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C32" s="138"/>
+      <c r="D32" s="138"/>
+      <c r="E32" s="138"/>
+      <c r="F32" s="138"/>
+      <c r="G32" s="138"/>
+      <c r="H32" s="138"/>
+      <c r="I32" s="138"/>
+      <c r="J32" s="138"/>
+      <c r="K32" s="149"/>
+    </row>
+    <row r="33" spans="2:11" ht="15" x14ac:dyDescent="0.45">
       <c r="B33" s="21"/>
       <c r="C33" s="133" t="s">
         <v>60</v>
@@ -6597,7 +6597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:11" ht="15" x14ac:dyDescent="0.4">
       <c r="B34" s="14" t="s">
         <v>2</v>
       </c>
@@ -6625,7 +6625,7 @@
       </c>
       <c r="K34" s="124"/>
     </row>
-    <row r="35" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:11" ht="14.35" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B35" s="51" t="str">
         <f>TEXT(Current_dref_E3+0.5*Current_rcav,"0.00")</f>
         <v>3.08</v>
@@ -6634,13 +6634,13 @@
         <f>Autodrive!L10*-100000000</f>
         <v>0</v>
       </c>
-      <c r="D35" s="3">
-        <f>Autodrive!M10*-100000000</f>
+      <c r="D35" s="3" t="str">
+        <f>IF(ABS(Autodrive!M10*-100000000)&gt;0,ABS(Autodrive!M10*-100000000)&gt;0,"")</f>
+        <v/>
+      </c>
+      <c r="E35" s="23">
+        <f>IFERROR(AVERAGE(C35:D35),"")</f>
         <v>0</v>
-      </c>
-      <c r="E35" s="23" t="str">
-        <f>IFERROR(AVERAGEIF(C35:D35,"&lt;&gt;0"),"")</f>
-        <v/>
       </c>
       <c r="F35" s="4" t="str">
         <f>IFERROR(E35*Current_Ppol_E3*Current_Pion_E3*Current_Pelec*CTP,"")</f>
@@ -6667,7 +6667,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B36" s="51" t="str">
         <f>TEXT(Current_R80_E3+0.5*Current_rcav,"0.00")</f>
         <v>4.45</v>
@@ -6676,13 +6676,13 @@
         <f>Autodrive!L11*-100000000</f>
         <v>0</v>
       </c>
-      <c r="D36" s="3">
-        <f>Autodrive!M11*-100000000</f>
+      <c r="D36" s="3" t="str">
+        <f>IF(ABS(Autodrive!M11*-100000000)&gt;0,ABS(Autodrive!M11*-100000000)&gt;0,"")</f>
+        <v/>
+      </c>
+      <c r="E36" s="23">
+        <f>IFERROR(AVERAGE(C36:D36),"")</f>
         <v>0</v>
-      </c>
-      <c r="E36" s="23" t="str">
-        <f>IFERROR(AVERAGEIF(C36:D36,"&lt;&gt;0"),"")</f>
-        <v/>
       </c>
       <c r="F36" s="4" t="str">
         <f>IFERROR(E36*Current_Ppol_E3*Current_Pion_E3*Current_Pelec*CTP,"")</f>
@@ -6703,25 +6703,25 @@
       </c>
       <c r="K36" s="95" t="str">
         <f>IF(ISNUMBER(E36),IFERROR(IF(AND(I36&gt;Current_LowETol_E1,I36&lt;Current_HighETol_E1),"PASSED","ENERGY FAIL"),""),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="130" t="str">
+        <v>ENERGY FAIL</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B37" s="137" t="str">
         <f>INDEX(Machines!A5:AF20,MATCH(MEASURE!H1,Machines,0),7)&amp;"E"</f>
         <v>15E</v>
       </c>
-      <c r="C37" s="131"/>
-      <c r="D37" s="131"/>
-      <c r="E37" s="131"/>
-      <c r="F37" s="131"/>
-      <c r="G37" s="131"/>
-      <c r="H37" s="131"/>
-      <c r="I37" s="131"/>
-      <c r="J37" s="131"/>
-      <c r="K37" s="132"/>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C37" s="138"/>
+      <c r="D37" s="138"/>
+      <c r="E37" s="138"/>
+      <c r="F37" s="138"/>
+      <c r="G37" s="138"/>
+      <c r="H37" s="138"/>
+      <c r="I37" s="138"/>
+      <c r="J37" s="138"/>
+      <c r="K37" s="149"/>
+    </row>
+    <row r="38" spans="2:11" ht="15" x14ac:dyDescent="0.45">
       <c r="B38" s="21"/>
       <c r="C38" s="133" t="s">
         <v>60</v>
@@ -6743,7 +6743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:11" ht="15" x14ac:dyDescent="0.4">
       <c r="B39" s="14" t="s">
         <v>2</v>
       </c>
@@ -6771,7 +6771,7 @@
       </c>
       <c r="K39" s="126"/>
     </row>
-    <row r="40" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:11" ht="14.35" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B40" s="51" t="str">
         <f>TEXT(Current_dref_E4+0.5*Current_rcav,"0.00")</f>
         <v>3.87</v>
@@ -6780,13 +6780,13 @@
         <f>Autodrive!L12*-100000000</f>
         <v>0</v>
       </c>
-      <c r="D40" s="3">
-        <f>Autodrive!M12*-100000000</f>
+      <c r="D40" s="3" t="str">
+        <f>IF(ABS(Autodrive!M12*-100000000)&gt;0,ABS(Autodrive!M12*-100000000)&gt;0,"")</f>
+        <v/>
+      </c>
+      <c r="E40" s="23">
+        <f>IFERROR(AVERAGE(C40:D40),"")</f>
         <v>0</v>
-      </c>
-      <c r="E40" s="23" t="str">
-        <f>IFERROR(AVERAGEIF(C40:D40,"&lt;&gt;0"),"")</f>
-        <v/>
       </c>
       <c r="F40" s="4" t="str">
         <f>IFERROR(E40*Current_Ppol_E4*Current_Pion_E4*Current_Pelec*CTP,"")</f>
@@ -6813,7 +6813,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B41" s="51" t="str">
         <f>TEXT(Current_R80_E4+0.5*Current_rcav,"0.00")</f>
         <v>5.55</v>
@@ -6822,13 +6822,13 @@
         <f>Autodrive!L13*-100000000</f>
         <v>0</v>
       </c>
-      <c r="D41" s="3">
-        <f>Autodrive!M13*-100000000</f>
+      <c r="D41" s="3" t="str">
+        <f>IF(ABS(Autodrive!M13*-100000000)&gt;0,ABS(Autodrive!M13*-100000000)&gt;0,"")</f>
+        <v/>
+      </c>
+      <c r="E41" s="23">
+        <f>IFERROR(AVERAGE(C41:D41),"")</f>
         <v>0</v>
-      </c>
-      <c r="E41" s="23" t="str">
-        <f>IFERROR(AVERAGEIF(C41:D41,"&lt;&gt;0"),"")</f>
-        <v/>
       </c>
       <c r="F41" s="4" t="str">
         <f>IFERROR(E41*Current_Ppol_E4*Current_Pion_E4*Current_Pelec*CTP,"")</f>
@@ -6849,25 +6849,25 @@
       </c>
       <c r="K41" s="95" t="str">
         <f>IF(ISNUMBER(E41),IFERROR(IF(AND(I41&gt;Current_LowETol_E1,I41&lt;Current_HighETol_E1),"PASSED","ENERGY FAIL"),""),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="42" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="130" t="str">
+        <v>ENERGY FAIL</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B42" s="137" t="str">
         <f>INDEX(Machines!A5:AF20,MATCH(MEASURE!H1,Machines,0),8)&amp;"E"</f>
         <v>18E</v>
       </c>
-      <c r="C42" s="131"/>
-      <c r="D42" s="131"/>
-      <c r="E42" s="131"/>
-      <c r="F42" s="131"/>
-      <c r="G42" s="131"/>
-      <c r="H42" s="131"/>
-      <c r="I42" s="131"/>
-      <c r="J42" s="131"/>
-      <c r="K42" s="132"/>
-    </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C42" s="138"/>
+      <c r="D42" s="138"/>
+      <c r="E42" s="138"/>
+      <c r="F42" s="138"/>
+      <c r="G42" s="138"/>
+      <c r="H42" s="138"/>
+      <c r="I42" s="138"/>
+      <c r="J42" s="138"/>
+      <c r="K42" s="149"/>
+    </row>
+    <row r="43" spans="2:11" ht="15" x14ac:dyDescent="0.45">
       <c r="B43" s="21"/>
       <c r="C43" s="133" t="s">
         <v>60</v>
@@ -6889,7 +6889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:11" ht="15" x14ac:dyDescent="0.4">
       <c r="B44" s="14" t="s">
         <v>2</v>
       </c>
@@ -6917,7 +6917,7 @@
       </c>
       <c r="K44" s="128"/>
     </row>
-    <row r="45" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:11" ht="14.35" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B45" s="51" t="str">
         <f>TEXT(Current_dref_E5+0.5*Current_rcav,"0.00")</f>
         <v>4.69</v>
@@ -6926,13 +6926,13 @@
         <f>Autodrive!L14*-100000000</f>
         <v>0</v>
       </c>
-      <c r="D45" s="3">
-        <f>Autodrive!M14*-100000000</f>
+      <c r="D45" s="3" t="str">
+        <f>IF(ABS(Autodrive!M14*-100000000)&gt;0,ABS(Autodrive!M14*-100000000)&gt;0,"")</f>
+        <v/>
+      </c>
+      <c r="E45" s="23">
+        <f>IFERROR(AVERAGE(C45:D45),"")</f>
         <v>0</v>
-      </c>
-      <c r="E45" s="23" t="str">
-        <f>IFERROR(AVERAGEIF(C45:D45,"&lt;&gt;0"),"")</f>
-        <v/>
       </c>
       <c r="F45" s="4" t="str">
         <f>IFERROR(E45*Current_Ppol_E5*Current_Pion_E5*Current_Pelec*CTP,"")</f>
@@ -6959,7 +6959,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B46" s="51" t="str">
         <f>TEXT(Current_R80_E5+0.5*Current_rcav,"0.00")</f>
         <v>6.55</v>
@@ -6968,13 +6968,13 @@
         <f>Autodrive!L15*-100000000</f>
         <v>0</v>
       </c>
-      <c r="D46" s="3">
-        <f>Autodrive!M15*-100000000</f>
+      <c r="D46" s="3" t="str">
+        <f>IF(ABS(Autodrive!M15*-100000000)&gt;0,ABS(Autodrive!M15*-100000000)&gt;0,"")</f>
+        <v/>
+      </c>
+      <c r="E46" s="23">
+        <f>IFERROR(AVERAGE(C46:D46),"")</f>
         <v>0</v>
-      </c>
-      <c r="E46" s="23" t="str">
-        <f>IFERROR(AVERAGEIF(C46:D46,"&lt;&gt;0"),"")</f>
-        <v/>
       </c>
       <c r="F46" s="4" t="str">
         <f>IFERROR(E46*Current_Ppol_E5*Current_Pion_E5*Current_Pelec*CTP,"")</f>
@@ -6995,26 +6995,11 @@
       </c>
       <c r="K46" s="95" t="str">
         <f>IF(ISNUMBER(E46),IFERROR(IF(AND(I46&gt;Current_LowETol_E1,I46&lt;Current_HighETol_E1),"PASSED","ENERGY FAIL"),""),"")</f>
-        <v/>
+        <v>ENERGY FAIL</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B1:G2"/>
-    <mergeCell ref="H1:K2"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="B21:K21"/>
-    <mergeCell ref="B10:K10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="B9:K9"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
     <mergeCell ref="B42:K42"/>
     <mergeCell ref="C43:E43"/>
     <mergeCell ref="G43:H43"/>
@@ -7031,6 +7016,21 @@
     <mergeCell ref="G38:H38"/>
     <mergeCell ref="C28:E28"/>
     <mergeCell ref="G28:H28"/>
+    <mergeCell ref="B1:G2"/>
+    <mergeCell ref="H1:K2"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="B21:K21"/>
+    <mergeCell ref="B10:K10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="B9:K9"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <conditionalFormatting sqref="K14">
     <cfRule type="cellIs" dxfId="23" priority="61" operator="notEqual">
@@ -7149,18 +7149,18 @@
       <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="31.25" customWidth="1"/>
-    <col min="2" max="2" width="10.625" customWidth="1"/>
-    <col min="3" max="3" width="12.125" customWidth="1"/>
+    <col min="1" max="1" width="31.21875" customWidth="1"/>
+    <col min="2" max="2" width="10.609375" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
-    <col min="14" max="14" width="15.125" customWidth="1"/>
-    <col min="20" max="20" width="29.375" customWidth="1"/>
-    <col min="21" max="21" width="4.125" customWidth="1"/>
+    <col min="14" max="14" width="15.109375" customWidth="1"/>
+    <col min="20" max="20" width="29.38671875" customWidth="1"/>
+    <col min="21" max="21" width="4.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="22.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="22" x14ac:dyDescent="0.4">
       <c r="A1" s="155" t="s">
         <v>49</v>
       </c>
@@ -7185,7 +7185,7 @@
       <c r="T1" s="155"/>
       <c r="U1" s="155"/>
     </row>
-    <row r="2" spans="1:21" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="17" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>33</v>
       </c>
@@ -7220,7 +7220,7 @@
       </c>
       <c r="U2" s="88"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A3" s="14"/>
       <c r="B3" s="9">
         <v>58</v>
@@ -7284,7 +7284,7 @@
       <c r="T3" s="89"/>
       <c r="U3" s="5"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A4" s="15" t="s">
         <v>65</v>
       </c>
@@ -7359,7 +7359,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
         <v>66</v>
       </c>
@@ -7434,7 +7434,7 @@
         <v>1854</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A6" s="15" t="s">
         <v>102</v>
       </c>
@@ -7509,7 +7509,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A7" s="15" t="s">
         <v>94</v>
       </c>
@@ -7584,7 +7584,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A8" s="15"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -7637,7 +7637,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A9" s="15"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -7690,7 +7690,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A10" s="15"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -7743,7 +7743,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A11" s="15"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -7796,7 +7796,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A12" s="15"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -7849,7 +7849,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A13" s="15"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -7902,7 +7902,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A14" s="15"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -7955,7 +7955,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A15" s="15"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -8008,7 +8008,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A16" s="15"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -8061,7 +8061,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A17" s="15"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -8114,7 +8114,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A18" s="15"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -8167,7 +8167,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A19" s="15"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -8220,7 +8220,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A20" s="15"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -8273,7 +8273,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A21" s="15"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -8375,15 +8375,15 @@
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="35.25" customWidth="1"/>
-    <col min="2" max="2" width="26.75" customWidth="1"/>
-    <col min="3" max="3" width="26.125" customWidth="1"/>
+    <col min="1" max="1" width="35.21875" customWidth="1"/>
+    <col min="2" max="2" width="26.71875" customWidth="1"/>
+    <col min="3" max="3" width="26.109375" customWidth="1"/>
     <col min="4" max="4" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="159" t="s">
         <v>107</v>
       </c>
@@ -8391,7 +8391,7 @@
       <c r="C1" s="160"/>
       <c r="D1" s="161"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="158" t="s">
         <v>68</v>
       </c>
@@ -8399,7 +8399,7 @@
       <c r="C2" s="158"/>
       <c r="D2" s="158"/>
     </row>
-    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>69</v>
       </c>
@@ -8411,7 +8411,7 @@
       </c>
       <c r="D3" s="88"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="15" t="s">
         <v>74</v>
       </c>
@@ -8426,7 +8426,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
         <v>75</v>
       </c>
@@ -8441,7 +8441,7 @@
         <v>1462</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" s="15" t="s">
         <v>104</v>
       </c>
@@ -8456,7 +8456,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" s="15"/>
       <c r="B7" s="3"/>
       <c r="C7" s="90"/>
@@ -8465,7 +8465,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" s="15"/>
       <c r="B8" s="3"/>
       <c r="C8" s="90"/>
@@ -8474,7 +8474,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" s="15"/>
       <c r="B9" s="3"/>
       <c r="C9" s="90"/>
@@ -8483,7 +8483,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" s="15"/>
       <c r="B10" s="3"/>
       <c r="C10" s="90"/>
@@ -8492,7 +8492,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" s="15"/>
       <c r="B11" s="3"/>
       <c r="C11" s="90"/>
@@ -8501,7 +8501,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12" s="15"/>
       <c r="B12" s="3"/>
       <c r="C12" s="90"/>
@@ -8510,7 +8510,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A13" s="15"/>
       <c r="B13" s="3"/>
       <c r="C13" s="90"/>
@@ -8519,7 +8519,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A14" s="15"/>
       <c r="B14" s="3"/>
       <c r="C14" s="90"/>
@@ -8528,7 +8528,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A15" s="15"/>
       <c r="B15" s="3"/>
       <c r="C15" s="90"/>
@@ -8537,7 +8537,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A16" s="15"/>
       <c r="B16" s="3"/>
       <c r="C16" s="90"/>
@@ -8546,7 +8546,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17" s="15"/>
       <c r="B17" s="3"/>
       <c r="C17" s="90"/>
@@ -8555,7 +8555,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A18" s="15"/>
       <c r="B18" s="3"/>
       <c r="C18" s="90"/>
@@ -8564,7 +8564,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19" s="15"/>
       <c r="B19" s="3"/>
       <c r="C19" s="90"/>
@@ -8573,7 +8573,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A20" s="15"/>
       <c r="B20" s="3"/>
       <c r="C20" s="90"/>
@@ -8582,7 +8582,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A21" s="15"/>
       <c r="B21" s="3"/>
       <c r="C21" s="90"/>
@@ -8591,7 +8591,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A22" s="15"/>
       <c r="B22" s="3"/>
       <c r="C22" s="90"/>
@@ -8600,7 +8600,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A23" s="15"/>
       <c r="B23" s="3"/>
       <c r="C23" s="90"/>
@@ -8609,7 +8609,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A24" s="15"/>
       <c r="B24" s="3"/>
       <c r="C24" s="90"/>
@@ -8655,310 +8655,310 @@
       <selection activeCell="BB25" sqref="BB25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="27.75" customWidth="1"/>
-    <col min="11" max="11" width="11.625" customWidth="1"/>
-    <col min="12" max="12" width="10.375" customWidth="1"/>
-    <col min="13" max="13" width="15.375" customWidth="1"/>
+    <col min="1" max="1" width="27.71875" customWidth="1"/>
+    <col min="11" max="11" width="11.609375" customWidth="1"/>
+    <col min="12" max="12" width="10.38671875" customWidth="1"/>
+    <col min="13" max="13" width="15.38671875" customWidth="1"/>
     <col min="14" max="14" width="14" customWidth="1"/>
-    <col min="15" max="15" width="9.25" customWidth="1"/>
+    <col min="15" max="15" width="9.21875" customWidth="1"/>
     <col min="16" max="16" width="16" customWidth="1"/>
-    <col min="17" max="17" width="14.125" customWidth="1"/>
-    <col min="43" max="43" width="8.875" customWidth="1"/>
-    <col min="44" max="44" width="11.125" customWidth="1"/>
-    <col min="45" max="45" width="10.375" customWidth="1"/>
-    <col min="46" max="46" width="9.75" customWidth="1"/>
-    <col min="47" max="47" width="10.25" customWidth="1"/>
+    <col min="17" max="17" width="14.109375" customWidth="1"/>
+    <col min="43" max="43" width="8.88671875" customWidth="1"/>
+    <col min="44" max="44" width="11.109375" customWidth="1"/>
+    <col min="45" max="45" width="10.38671875" customWidth="1"/>
+    <col min="46" max="46" width="9.71875" customWidth="1"/>
+    <col min="47" max="47" width="10.21875" customWidth="1"/>
     <col min="49" max="49" width="9" customWidth="1"/>
-    <col min="50" max="50" width="9.125" customWidth="1"/>
-    <col min="77" max="77" width="16.625" customWidth="1"/>
+    <col min="50" max="50" width="9.109375" customWidth="1"/>
+    <col min="77" max="77" width="16.609375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="162" t="s">
+    <row r="1" spans="1:77" ht="22" x14ac:dyDescent="0.4">
+      <c r="A1" s="170" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="162"/>
-      <c r="C1" s="162"/>
-      <c r="D1" s="162"/>
-      <c r="E1" s="162"/>
-      <c r="F1" s="162"/>
-      <c r="G1" s="162"/>
-      <c r="H1" s="162"/>
-      <c r="I1" s="162"/>
-      <c r="J1" s="162"/>
-      <c r="K1" s="162"/>
-      <c r="L1" s="162"/>
-      <c r="M1" s="162"/>
-      <c r="N1" s="162"/>
-      <c r="O1" s="162"/>
-      <c r="P1" s="162"/>
-      <c r="Q1" s="162"/>
-      <c r="R1" s="162"/>
-      <c r="S1" s="162"/>
-      <c r="T1" s="162"/>
-      <c r="U1" s="162"/>
-      <c r="V1" s="162"/>
-      <c r="W1" s="162"/>
-      <c r="X1" s="162"/>
-      <c r="Y1" s="162"/>
-      <c r="Z1" s="162"/>
-      <c r="AA1" s="162"/>
-      <c r="AB1" s="162"/>
-      <c r="AC1" s="162"/>
-      <c r="AD1" s="162"/>
-      <c r="AE1" s="162"/>
-      <c r="AF1" s="162"/>
-      <c r="AG1" s="162"/>
-      <c r="AH1" s="162"/>
-      <c r="AI1" s="162"/>
-      <c r="AJ1" s="162"/>
-      <c r="AK1" s="162"/>
-      <c r="AL1" s="162"/>
-      <c r="AM1" s="162"/>
-      <c r="AN1" s="162"/>
-      <c r="AO1" s="162"/>
-      <c r="AP1" s="162"/>
-      <c r="AQ1" s="162"/>
-      <c r="AR1" s="162"/>
-      <c r="AS1" s="162"/>
-      <c r="AT1" s="162"/>
-      <c r="AU1" s="162"/>
-      <c r="AV1" s="162"/>
-      <c r="AW1" s="162"/>
-      <c r="AX1" s="162"/>
-      <c r="AY1" s="162"/>
-      <c r="AZ1" s="162"/>
-      <c r="BA1" s="162"/>
-      <c r="BB1" s="162"/>
-      <c r="BC1" s="162"/>
-      <c r="BD1" s="162"/>
-      <c r="BE1" s="162"/>
-      <c r="BF1" s="162"/>
-      <c r="BG1" s="162"/>
-      <c r="BH1" s="162"/>
-      <c r="BI1" s="162"/>
-      <c r="BJ1" s="162"/>
-      <c r="BK1" s="162"/>
-      <c r="BL1" s="162"/>
-      <c r="BM1" s="162"/>
-      <c r="BN1" s="162"/>
-      <c r="BO1" s="162"/>
-      <c r="BP1" s="162"/>
-      <c r="BQ1" s="162"/>
-      <c r="BR1" s="162"/>
-      <c r="BS1" s="162"/>
-      <c r="BT1" s="162"/>
-      <c r="BU1" s="162"/>
-      <c r="BV1" s="162"/>
-      <c r="BW1" s="162"/>
-      <c r="BX1" s="162"/>
-      <c r="BY1" s="162"/>
-    </row>
-    <row r="2" spans="1:77" x14ac:dyDescent="0.3">
-      <c r="A2" s="176" t="s">
+      <c r="B1" s="170"/>
+      <c r="C1" s="170"/>
+      <c r="D1" s="170"/>
+      <c r="E1" s="170"/>
+      <c r="F1" s="170"/>
+      <c r="G1" s="170"/>
+      <c r="H1" s="170"/>
+      <c r="I1" s="170"/>
+      <c r="J1" s="170"/>
+      <c r="K1" s="170"/>
+      <c r="L1" s="170"/>
+      <c r="M1" s="170"/>
+      <c r="N1" s="170"/>
+      <c r="O1" s="170"/>
+      <c r="P1" s="170"/>
+      <c r="Q1" s="170"/>
+      <c r="R1" s="170"/>
+      <c r="S1" s="170"/>
+      <c r="T1" s="170"/>
+      <c r="U1" s="170"/>
+      <c r="V1" s="170"/>
+      <c r="W1" s="170"/>
+      <c r="X1" s="170"/>
+      <c r="Y1" s="170"/>
+      <c r="Z1" s="170"/>
+      <c r="AA1" s="170"/>
+      <c r="AB1" s="170"/>
+      <c r="AC1" s="170"/>
+      <c r="AD1" s="170"/>
+      <c r="AE1" s="170"/>
+      <c r="AF1" s="170"/>
+      <c r="AG1" s="170"/>
+      <c r="AH1" s="170"/>
+      <c r="AI1" s="170"/>
+      <c r="AJ1" s="170"/>
+      <c r="AK1" s="170"/>
+      <c r="AL1" s="170"/>
+      <c r="AM1" s="170"/>
+      <c r="AN1" s="170"/>
+      <c r="AO1" s="170"/>
+      <c r="AP1" s="170"/>
+      <c r="AQ1" s="170"/>
+      <c r="AR1" s="170"/>
+      <c r="AS1" s="170"/>
+      <c r="AT1" s="170"/>
+      <c r="AU1" s="170"/>
+      <c r="AV1" s="170"/>
+      <c r="AW1" s="170"/>
+      <c r="AX1" s="170"/>
+      <c r="AY1" s="170"/>
+      <c r="AZ1" s="170"/>
+      <c r="BA1" s="170"/>
+      <c r="BB1" s="170"/>
+      <c r="BC1" s="170"/>
+      <c r="BD1" s="170"/>
+      <c r="BE1" s="170"/>
+      <c r="BF1" s="170"/>
+      <c r="BG1" s="170"/>
+      <c r="BH1" s="170"/>
+      <c r="BI1" s="170"/>
+      <c r="BJ1" s="170"/>
+      <c r="BK1" s="170"/>
+      <c r="BL1" s="170"/>
+      <c r="BM1" s="170"/>
+      <c r="BN1" s="170"/>
+      <c r="BO1" s="170"/>
+      <c r="BP1" s="170"/>
+      <c r="BQ1" s="170"/>
+      <c r="BR1" s="170"/>
+      <c r="BS1" s="170"/>
+      <c r="BT1" s="170"/>
+      <c r="BU1" s="170"/>
+      <c r="BV1" s="170"/>
+      <c r="BW1" s="170"/>
+      <c r="BX1" s="170"/>
+      <c r="BY1" s="170"/>
+    </row>
+    <row r="2" spans="1:77" x14ac:dyDescent="0.4">
+      <c r="A2" s="164" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="176"/>
-      <c r="H2" s="177"/>
-      <c r="I2" s="172" t="s">
+      <c r="B2" s="164"/>
+      <c r="C2" s="164"/>
+      <c r="D2" s="164"/>
+      <c r="E2" s="164"/>
+      <c r="F2" s="164"/>
+      <c r="G2" s="164"/>
+      <c r="H2" s="165"/>
+      <c r="I2" s="179" t="s">
         <v>83</v>
       </c>
-      <c r="J2" s="173"/>
-      <c r="K2" s="173"/>
-      <c r="L2" s="173"/>
-      <c r="M2" s="173"/>
-      <c r="N2" s="173"/>
-      <c r="O2" s="173"/>
-      <c r="P2" s="173"/>
-      <c r="Q2" s="174"/>
-      <c r="R2" s="178" t="s">
+      <c r="J2" s="180"/>
+      <c r="K2" s="180"/>
+      <c r="L2" s="180"/>
+      <c r="M2" s="180"/>
+      <c r="N2" s="180"/>
+      <c r="O2" s="180"/>
+      <c r="P2" s="180"/>
+      <c r="Q2" s="181"/>
+      <c r="R2" s="166" t="s">
         <v>85</v>
       </c>
-      <c r="S2" s="178"/>
-      <c r="T2" s="178"/>
-      <c r="U2" s="178"/>
-      <c r="V2" s="178"/>
-      <c r="W2" s="178"/>
-      <c r="X2" s="178"/>
-      <c r="Y2" s="178"/>
-      <c r="Z2" s="178"/>
-      <c r="AA2" s="178"/>
-      <c r="AB2" s="178"/>
-      <c r="AC2" s="178"/>
-      <c r="AD2" s="178"/>
-      <c r="AE2" s="178"/>
-      <c r="AF2" s="178"/>
-      <c r="AG2" s="178"/>
-      <c r="AH2" s="178"/>
-      <c r="AI2" s="178"/>
-      <c r="AJ2" s="178"/>
-      <c r="AK2" s="178"/>
-      <c r="AL2" s="178"/>
-      <c r="AM2" s="178"/>
-      <c r="AN2" s="178"/>
-      <c r="AO2" s="178"/>
-      <c r="AP2" s="178"/>
-      <c r="AQ2" s="178"/>
-      <c r="AR2" s="178"/>
-      <c r="AS2" s="178"/>
-      <c r="AT2" s="178"/>
-      <c r="AU2" s="178"/>
-      <c r="AV2" s="178"/>
-      <c r="AW2" s="178"/>
-      <c r="AX2" s="178"/>
-      <c r="AY2" s="178"/>
-      <c r="AZ2" s="178"/>
-      <c r="BA2" s="178"/>
-      <c r="BB2" s="178"/>
-      <c r="BC2" s="178"/>
-      <c r="BD2" s="178"/>
-      <c r="BE2" s="179"/>
-      <c r="BF2" s="180" t="s">
+      <c r="S2" s="166"/>
+      <c r="T2" s="166"/>
+      <c r="U2" s="166"/>
+      <c r="V2" s="166"/>
+      <c r="W2" s="166"/>
+      <c r="X2" s="166"/>
+      <c r="Y2" s="166"/>
+      <c r="Z2" s="166"/>
+      <c r="AA2" s="166"/>
+      <c r="AB2" s="166"/>
+      <c r="AC2" s="166"/>
+      <c r="AD2" s="166"/>
+      <c r="AE2" s="166"/>
+      <c r="AF2" s="166"/>
+      <c r="AG2" s="166"/>
+      <c r="AH2" s="166"/>
+      <c r="AI2" s="166"/>
+      <c r="AJ2" s="166"/>
+      <c r="AK2" s="166"/>
+      <c r="AL2" s="166"/>
+      <c r="AM2" s="166"/>
+      <c r="AN2" s="166"/>
+      <c r="AO2" s="166"/>
+      <c r="AP2" s="166"/>
+      <c r="AQ2" s="166"/>
+      <c r="AR2" s="166"/>
+      <c r="AS2" s="166"/>
+      <c r="AT2" s="166"/>
+      <c r="AU2" s="166"/>
+      <c r="AV2" s="166"/>
+      <c r="AW2" s="166"/>
+      <c r="AX2" s="166"/>
+      <c r="AY2" s="166"/>
+      <c r="AZ2" s="166"/>
+      <c r="BA2" s="166"/>
+      <c r="BB2" s="166"/>
+      <c r="BC2" s="166"/>
+      <c r="BD2" s="166"/>
+      <c r="BE2" s="167"/>
+      <c r="BF2" s="168" t="s">
         <v>86</v>
       </c>
-      <c r="BG2" s="181"/>
-      <c r="BH2" s="181"/>
-      <c r="BI2" s="181"/>
-      <c r="BJ2" s="181"/>
-      <c r="BK2" s="181"/>
-      <c r="BL2" s="181"/>
-      <c r="BM2" s="181"/>
-      <c r="BN2" s="181"/>
-      <c r="BO2" s="181"/>
-      <c r="BP2" s="181"/>
-      <c r="BQ2" s="181"/>
-      <c r="BR2" s="181"/>
-      <c r="BS2" s="181"/>
-      <c r="BT2" s="181"/>
-      <c r="BU2" s="181"/>
-      <c r="BV2" s="181"/>
-      <c r="BW2" s="181"/>
-      <c r="BX2" s="181"/>
-      <c r="BY2" s="163" t="s">
+      <c r="BG2" s="169"/>
+      <c r="BH2" s="169"/>
+      <c r="BI2" s="169"/>
+      <c r="BJ2" s="169"/>
+      <c r="BK2" s="169"/>
+      <c r="BL2" s="169"/>
+      <c r="BM2" s="169"/>
+      <c r="BN2" s="169"/>
+      <c r="BO2" s="169"/>
+      <c r="BP2" s="169"/>
+      <c r="BQ2" s="169"/>
+      <c r="BR2" s="169"/>
+      <c r="BS2" s="169"/>
+      <c r="BT2" s="169"/>
+      <c r="BU2" s="169"/>
+      <c r="BV2" s="169"/>
+      <c r="BW2" s="169"/>
+      <c r="BX2" s="169"/>
+      <c r="BY2" s="171" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:77" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:77" ht="17" x14ac:dyDescent="0.4">
       <c r="A3" s="60"/>
-      <c r="B3" s="166" t="s">
+      <c r="B3" s="174" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="166"/>
-      <c r="D3" s="166"/>
-      <c r="E3" s="166"/>
-      <c r="F3" s="166"/>
-      <c r="G3" s="166"/>
-      <c r="H3" s="169"/>
+      <c r="C3" s="174"/>
+      <c r="D3" s="174"/>
+      <c r="E3" s="174"/>
+      <c r="F3" s="174"/>
+      <c r="G3" s="174"/>
+      <c r="H3" s="177"/>
       <c r="I3" s="156" t="s">
         <v>30</v>
       </c>
       <c r="J3" s="157"/>
-      <c r="K3" s="168" t="s">
+      <c r="K3" s="176" t="s">
         <v>78</v>
       </c>
       <c r="L3" s="157"/>
-      <c r="M3" s="168" t="s">
+      <c r="M3" s="176" t="s">
         <v>79</v>
       </c>
-      <c r="N3" s="167"/>
+      <c r="N3" s="175"/>
       <c r="O3" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="P3" s="168" t="s">
+      <c r="P3" s="176" t="s">
         <v>56</v>
       </c>
-      <c r="Q3" s="169"/>
-      <c r="R3" s="171" t="s">
+      <c r="Q3" s="177"/>
+      <c r="R3" s="178" t="s">
         <v>48</v>
       </c>
-      <c r="S3" s="131"/>
-      <c r="T3" s="131"/>
-      <c r="U3" s="131"/>
-      <c r="V3" s="170"/>
-      <c r="W3" s="130" t="s">
+      <c r="S3" s="138"/>
+      <c r="T3" s="138"/>
+      <c r="U3" s="138"/>
+      <c r="V3" s="162"/>
+      <c r="W3" s="137" t="s">
         <v>15</v>
       </c>
-      <c r="X3" s="131"/>
-      <c r="Y3" s="131"/>
-      <c r="Z3" s="131"/>
+      <c r="X3" s="138"/>
+      <c r="Y3" s="138"/>
+      <c r="Z3" s="138"/>
       <c r="AA3" s="156"/>
       <c r="AB3" s="157" t="s">
         <v>47</v>
       </c>
-      <c r="AC3" s="131"/>
-      <c r="AD3" s="131"/>
-      <c r="AE3" s="131"/>
-      <c r="AF3" s="170"/>
-      <c r="AG3" s="130" t="s">
+      <c r="AC3" s="138"/>
+      <c r="AD3" s="138"/>
+      <c r="AE3" s="138"/>
+      <c r="AF3" s="162"/>
+      <c r="AG3" s="137" t="s">
         <v>99</v>
       </c>
-      <c r="AH3" s="131"/>
-      <c r="AI3" s="131"/>
-      <c r="AJ3" s="131"/>
-      <c r="AK3" s="170"/>
-      <c r="AL3" s="130" t="s">
+      <c r="AH3" s="138"/>
+      <c r="AI3" s="138"/>
+      <c r="AJ3" s="138"/>
+      <c r="AK3" s="162"/>
+      <c r="AL3" s="137" t="s">
         <v>100</v>
       </c>
-      <c r="AM3" s="131"/>
-      <c r="AN3" s="131"/>
-      <c r="AO3" s="131"/>
-      <c r="AP3" s="170"/>
-      <c r="AQ3" s="130" t="s">
+      <c r="AM3" s="138"/>
+      <c r="AN3" s="138"/>
+      <c r="AO3" s="138"/>
+      <c r="AP3" s="162"/>
+      <c r="AQ3" s="137" t="s">
         <v>126</v>
       </c>
-      <c r="AR3" s="131"/>
-      <c r="AS3" s="131"/>
-      <c r="AT3" s="131"/>
-      <c r="AU3" s="170"/>
-      <c r="AV3" s="130" t="s">
+      <c r="AR3" s="138"/>
+      <c r="AS3" s="138"/>
+      <c r="AT3" s="138"/>
+      <c r="AU3" s="162"/>
+      <c r="AV3" s="137" t="s">
         <v>127</v>
       </c>
-      <c r="AW3" s="131"/>
-      <c r="AX3" s="131"/>
-      <c r="AY3" s="131"/>
-      <c r="AZ3" s="170"/>
-      <c r="BA3" s="130" t="s">
+      <c r="AW3" s="138"/>
+      <c r="AX3" s="138"/>
+      <c r="AY3" s="138"/>
+      <c r="AZ3" s="162"/>
+      <c r="BA3" s="137" t="s">
         <v>128</v>
       </c>
-      <c r="BB3" s="131"/>
-      <c r="BC3" s="131"/>
-      <c r="BD3" s="131"/>
-      <c r="BE3" s="170"/>
-      <c r="BF3" s="130" t="s">
+      <c r="BB3" s="138"/>
+      <c r="BC3" s="138"/>
+      <c r="BD3" s="138"/>
+      <c r="BE3" s="162"/>
+      <c r="BF3" s="137" t="s">
         <v>77</v>
       </c>
-      <c r="BG3" s="131"/>
-      <c r="BH3" s="131"/>
-      <c r="BI3" s="131"/>
-      <c r="BJ3" s="175"/>
+      <c r="BG3" s="138"/>
+      <c r="BH3" s="138"/>
+      <c r="BI3" s="138"/>
+      <c r="BJ3" s="163"/>
       <c r="BK3" s="156" t="s">
         <v>4</v>
       </c>
-      <c r="BL3" s="166"/>
-      <c r="BM3" s="166"/>
-      <c r="BN3" s="166"/>
-      <c r="BO3" s="166"/>
-      <c r="BP3" s="166"/>
-      <c r="BQ3" s="167"/>
-      <c r="BR3" s="168" t="s">
+      <c r="BL3" s="174"/>
+      <c r="BM3" s="174"/>
+      <c r="BN3" s="174"/>
+      <c r="BO3" s="174"/>
+      <c r="BP3" s="174"/>
+      <c r="BQ3" s="175"/>
+      <c r="BR3" s="176" t="s">
         <v>14</v>
       </c>
-      <c r="BS3" s="166"/>
-      <c r="BT3" s="166"/>
-      <c r="BU3" s="166"/>
-      <c r="BV3" s="166"/>
-      <c r="BW3" s="166"/>
-      <c r="BX3" s="167"/>
-      <c r="BY3" s="164"/>
-    </row>
-    <row r="4" spans="1:77" x14ac:dyDescent="0.3">
+      <c r="BS3" s="174"/>
+      <c r="BT3" s="174"/>
+      <c r="BU3" s="174"/>
+      <c r="BV3" s="174"/>
+      <c r="BW3" s="174"/>
+      <c r="BX3" s="175"/>
+      <c r="BY3" s="172"/>
+    </row>
+    <row r="4" spans="1:77" ht="15" x14ac:dyDescent="0.45">
       <c r="A4" s="61" t="s">
         <v>34</v>
       </c>
@@ -9187,9 +9187,9 @@
       <c r="BX4" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="BY4" s="165"/>
-    </row>
-    <row r="5" spans="1:77" x14ac:dyDescent="0.3">
+      <c r="BY4" s="173"/>
+    </row>
+    <row r="5" spans="1:77" x14ac:dyDescent="0.4">
       <c r="A5" s="70" t="s">
         <v>36</v>
       </c>
@@ -9437,7 +9437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:77" x14ac:dyDescent="0.4">
       <c r="A6" s="70" t="s">
         <v>35</v>
       </c>
@@ -9685,7 +9685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:77" x14ac:dyDescent="0.4">
       <c r="A7" s="70" t="s">
         <v>98</v>
       </c>
@@ -9933,7 +9933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:77" x14ac:dyDescent="0.4">
       <c r="A8" s="70"/>
       <c r="B8" s="71"/>
       <c r="C8" s="71"/>
@@ -10057,7 +10057,7 @@
       <c r="BX8" s="43"/>
       <c r="BY8" s="43"/>
     </row>
-    <row r="9" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:77" x14ac:dyDescent="0.4">
       <c r="A9" s="70"/>
       <c r="B9" s="71"/>
       <c r="C9" s="71"/>
@@ -10181,7 +10181,7 @@
       <c r="BX9" s="43"/>
       <c r="BY9" s="43"/>
     </row>
-    <row r="10" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:77" x14ac:dyDescent="0.4">
       <c r="A10" s="70"/>
       <c r="B10" s="71"/>
       <c r="C10" s="71"/>
@@ -10305,7 +10305,7 @@
       <c r="BX10" s="43"/>
       <c r="BY10" s="43"/>
     </row>
-    <row r="11" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:77" x14ac:dyDescent="0.4">
       <c r="A11" s="70"/>
       <c r="B11" s="71"/>
       <c r="C11" s="71"/>
@@ -10429,7 +10429,7 @@
       <c r="BX11" s="43"/>
       <c r="BY11" s="43"/>
     </row>
-    <row r="12" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:77" x14ac:dyDescent="0.4">
       <c r="A12" s="70"/>
       <c r="B12" s="71"/>
       <c r="C12" s="71"/>
@@ -10553,7 +10553,7 @@
       <c r="BX12" s="43"/>
       <c r="BY12" s="43"/>
     </row>
-    <row r="13" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:77" x14ac:dyDescent="0.4">
       <c r="A13" s="70"/>
       <c r="B13" s="71"/>
       <c r="C13" s="71"/>
@@ -10677,7 +10677,7 @@
       <c r="BX13" s="43"/>
       <c r="BY13" s="43"/>
     </row>
-    <row r="14" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:77" x14ac:dyDescent="0.4">
       <c r="A14" s="70"/>
       <c r="B14" s="71"/>
       <c r="C14" s="71"/>
@@ -10801,7 +10801,7 @@
       <c r="BX14" s="43"/>
       <c r="BY14" s="43"/>
     </row>
-    <row r="15" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:77" x14ac:dyDescent="0.4">
       <c r="A15" s="70"/>
       <c r="B15" s="71"/>
       <c r="C15" s="71"/>
@@ -10925,7 +10925,7 @@
       <c r="BX15" s="43"/>
       <c r="BY15" s="43"/>
     </row>
-    <row r="16" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:77" x14ac:dyDescent="0.4">
       <c r="A16" s="70"/>
       <c r="B16" s="71"/>
       <c r="C16" s="71"/>
@@ -11049,7 +11049,7 @@
       <c r="BX16" s="43"/>
       <c r="BY16" s="43"/>
     </row>
-    <row r="17" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:77" x14ac:dyDescent="0.4">
       <c r="A17" s="70"/>
       <c r="B17" s="71"/>
       <c r="C17" s="71"/>
@@ -11173,7 +11173,7 @@
       <c r="BX17" s="43"/>
       <c r="BY17" s="43"/>
     </row>
-    <row r="18" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:77" x14ac:dyDescent="0.4">
       <c r="A18" s="70"/>
       <c r="B18" s="71"/>
       <c r="C18" s="71"/>
@@ -11297,7 +11297,7 @@
       <c r="BX18" s="43"/>
       <c r="BY18" s="43"/>
     </row>
-    <row r="19" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:77" x14ac:dyDescent="0.4">
       <c r="A19" s="70"/>
       <c r="B19" s="71"/>
       <c r="C19" s="71"/>
@@ -11421,7 +11421,7 @@
       <c r="BX19" s="43"/>
       <c r="BY19" s="43"/>
     </row>
-    <row r="20" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:77" x14ac:dyDescent="0.4">
       <c r="A20" s="70"/>
       <c r="B20" s="71"/>
       <c r="C20" s="71"/>
@@ -11547,12 +11547,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="AQ3:AU3"/>
-    <mergeCell ref="BF3:BJ3"/>
-    <mergeCell ref="AV3:AZ3"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="R2:BE2"/>
-    <mergeCell ref="BF2:BX2"/>
     <mergeCell ref="A1:BY1"/>
     <mergeCell ref="BY2:BY4"/>
     <mergeCell ref="BK3:BQ3"/>
@@ -11569,6 +11563,12 @@
     <mergeCell ref="W3:AA3"/>
     <mergeCell ref="AB3:AF3"/>
     <mergeCell ref="I2:Q2"/>
+    <mergeCell ref="AQ3:AU3"/>
+    <mergeCell ref="BF3:BJ3"/>
+    <mergeCell ref="AV3:AZ3"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="R2:BE2"/>
+    <mergeCell ref="BF2:BX2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -11586,96 +11586,96 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="33.625" customWidth="1"/>
-    <col min="2" max="2" width="37.25" customWidth="1"/>
+    <col min="1" max="1" width="33.609375" customWidth="1"/>
+    <col min="2" max="2" width="37.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="116.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="116.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="113" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" s="112" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A11" s="3"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A12" s="3"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A13" s="3"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A14" s="3"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A16" s="3"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A17" s="3"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A18" s="3"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A19" s="3"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A20" s="3"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A21" s="3"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A22" s="3"/>
     </row>
   </sheetData>
@@ -11696,21 +11696,21 @@
       <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.375" customWidth="1"/>
-    <col min="2" max="2" width="11.75" customWidth="1"/>
-    <col min="3" max="3" width="10.875" customWidth="1"/>
-    <col min="4" max="4" width="12.625" customWidth="1"/>
-    <col min="10" max="10" width="12.875" customWidth="1"/>
-    <col min="11" max="11" width="24.125" customWidth="1"/>
+    <col min="1" max="1" width="10.38671875" customWidth="1"/>
+    <col min="2" max="2" width="11.71875" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" customWidth="1"/>
+    <col min="4" max="4" width="12.609375" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" customWidth="1"/>
+    <col min="11" max="11" width="24.109375" customWidth="1"/>
     <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="14" max="14" width="8.875" customWidth="1"/>
-    <col min="15" max="15" width="12.25" customWidth="1"/>
-    <col min="16" max="16" width="17.375" customWidth="1"/>
+    <col min="14" max="14" width="8.88671875" customWidth="1"/>
+    <col min="15" max="15" width="12.21875" customWidth="1"/>
+    <col min="16" max="16" width="17.38671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="159" t="s">
         <v>105</v>
       </c>
@@ -11730,46 +11730,46 @@
       <c r="O1" s="160"/>
       <c r="P1" s="161"/>
     </row>
-    <row r="2" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="191" t="s">
+    <row r="2" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="194" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="191"/>
-      <c r="C2" s="191"/>
-      <c r="D2" s="191"/>
-      <c r="E2" s="191"/>
-      <c r="F2" s="191"/>
-      <c r="G2" s="191"/>
-      <c r="H2" s="191"/>
-      <c r="I2" s="191"/>
-      <c r="J2" s="191"/>
-    </row>
-    <row r="3" spans="1:16" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="187" t="s">
+      <c r="B2" s="194"/>
+      <c r="C2" s="194"/>
+      <c r="D2" s="194"/>
+      <c r="E2" s="194"/>
+      <c r="F2" s="194"/>
+      <c r="G2" s="194"/>
+      <c r="H2" s="194"/>
+      <c r="I2" s="194"/>
+      <c r="J2" s="194"/>
+    </row>
+    <row r="3" spans="1:16" ht="17" x14ac:dyDescent="0.4">
+      <c r="A3" s="186" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="188"/>
-      <c r="C3" s="188"/>
-      <c r="D3" s="188"/>
-      <c r="E3" s="189"/>
-      <c r="F3" s="187" t="s">
+      <c r="B3" s="187"/>
+      <c r="C3" s="187"/>
+      <c r="D3" s="187"/>
+      <c r="E3" s="193"/>
+      <c r="F3" s="186" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="188"/>
-      <c r="H3" s="188"/>
-      <c r="I3" s="188"/>
-      <c r="J3" s="194"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="185" t="str">
+      <c r="G3" s="187"/>
+      <c r="H3" s="187"/>
+      <c r="I3" s="187"/>
+      <c r="J3" s="188"/>
+    </row>
+    <row r="4" spans="1:16" ht="15" x14ac:dyDescent="0.45">
+      <c r="A4" s="189" t="str">
         <f>INDEX(Machines!A5:AF20,MATCH(MEASURE!H1,Machines,0),2)&amp;"X"</f>
         <v>6X</v>
       </c>
       <c r="B4" s="133"/>
       <c r="C4" s="133"/>
       <c r="D4" s="133"/>
-      <c r="E4" s="190"/>
-      <c r="F4" s="185" t="str">
+      <c r="E4" s="192"/>
+      <c r="F4" s="189" t="str">
         <f>INDEX(Machines!A5:AF20,MATCH(MEASURE!H1,Machines,0),2)&amp;"X"</f>
         <v>6X</v>
       </c>
@@ -11778,7 +11778,7 @@
       <c r="I4" s="133"/>
       <c r="J4" s="133"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A5" s="14" t="s">
         <v>5</v>
       </c>
@@ -11806,7 +11806,7 @@
       </c>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A6" s="14">
         <v>150</v>
       </c>
@@ -11820,7 +11820,7 @@
         <f>IFERROR(AVERAGE(B6:C6),"")</f>
         <v>26.65</v>
       </c>
-      <c r="E6" s="182">
+      <c r="E6" s="184">
         <f>(1-A7/A6)/(D7/D6-A7/A6)</f>
         <v>1.0037664783427496</v>
       </c>
@@ -11837,12 +11837,12 @@
         <f>IFERROR(AVERAGE(G6:H6),"")</f>
         <v>26.75</v>
       </c>
-      <c r="J6" s="182">
+      <c r="J6" s="184">
         <f>(I6+I7)/(2*I6)</f>
         <v>1.0011214953271028</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A7" s="14">
         <v>300</v>
       </c>
@@ -11856,7 +11856,7 @@
         <f>IFERROR(AVERAGE(B7:C7),"")</f>
         <v>26.75</v>
       </c>
-      <c r="E7" s="182"/>
+      <c r="E7" s="184"/>
       <c r="F7" s="14">
         <v>300</v>
       </c>
@@ -11870,27 +11870,27 @@
         <f>IFERROR(AVERAGE(G7:H7),"")</f>
         <v>26.81</v>
       </c>
-      <c r="J7" s="182"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="183" t="str">
+      <c r="J7" s="184"/>
+    </row>
+    <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.45">
+      <c r="A8" s="182" t="str">
         <f>INDEX(Machines!A5:AF20,MATCH(MEASURE!H1,Machines,0),3)&amp;"X"</f>
         <v>15X</v>
       </c>
-      <c r="B8" s="184"/>
-      <c r="C8" s="184"/>
-      <c r="D8" s="184"/>
-      <c r="E8" s="186"/>
-      <c r="F8" s="183" t="str">
+      <c r="B8" s="183"/>
+      <c r="C8" s="183"/>
+      <c r="D8" s="183"/>
+      <c r="E8" s="185"/>
+      <c r="F8" s="182" t="str">
         <f>INDEX(Machines!A5:AF20,MATCH(MEASURE!H1,Machines,0),3)&amp;"X"</f>
         <v>15X</v>
       </c>
-      <c r="G8" s="184"/>
-      <c r="H8" s="184"/>
-      <c r="I8" s="184"/>
-      <c r="J8" s="184"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G8" s="183"/>
+      <c r="H8" s="183"/>
+      <c r="I8" s="183"/>
+      <c r="J8" s="183"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A9" s="14" t="s">
         <v>5</v>
       </c>
@@ -11918,7 +11918,7 @@
       </c>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A10" s="14">
         <v>150</v>
       </c>
@@ -11932,7 +11932,7 @@
         <f>IFERROR(AVERAGE(B10:C10),"")</f>
         <v>30.2</v>
       </c>
-      <c r="E10" s="182">
+      <c r="E10" s="184">
         <f>(1-A11/A10)/(D11/D10-A11/A10)</f>
         <v>1.0063312229256915</v>
       </c>
@@ -11949,12 +11949,12 @@
         <f>IFERROR(AVERAGE(G10:H10),"")</f>
         <v>30.39</v>
       </c>
-      <c r="J10" s="182">
+      <c r="J10" s="184">
         <f>(I10+I11)/(2*I10)</f>
         <v>1.0009871668311945</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A11" s="14">
         <v>300</v>
       </c>
@@ -11968,7 +11968,7 @@
         <f>IFERROR(AVERAGE(B11:C11),"")</f>
         <v>30.39</v>
       </c>
-      <c r="E11" s="182"/>
+      <c r="E11" s="184"/>
       <c r="F11" s="14">
         <v>300</v>
       </c>
@@ -11982,25 +11982,25 @@
         <f>IFERROR(AVERAGE(G11:H11),"")</f>
         <v>30.45</v>
       </c>
-      <c r="J11" s="182"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="183" t="s">
+      <c r="J11" s="184"/>
+    </row>
+    <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.45">
+      <c r="A12" s="182" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="184"/>
-      <c r="C12" s="184"/>
-      <c r="D12" s="184"/>
-      <c r="E12" s="186"/>
-      <c r="F12" s="183" t="s">
+      <c r="B12" s="183"/>
+      <c r="C12" s="183"/>
+      <c r="D12" s="183"/>
+      <c r="E12" s="185"/>
+      <c r="F12" s="182" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="184"/>
-      <c r="H12" s="184"/>
-      <c r="I12" s="184"/>
-      <c r="J12" s="184"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G12" s="183"/>
+      <c r="H12" s="183"/>
+      <c r="I12" s="183"/>
+      <c r="J12" s="183"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A13" s="14" t="s">
         <v>5</v>
       </c>
@@ -12028,7 +12028,7 @@
       </c>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A14" s="14">
         <v>150</v>
       </c>
@@ -12042,7 +12042,7 @@
         <f>IFERROR(AVERAGE(B14:C14),"")</f>
         <v>42.284999999999997</v>
       </c>
-      <c r="E14" s="182">
+      <c r="E14" s="184">
         <f>(1-A15/A14)/(D15/D14-A15/A14)</f>
         <v>1.0141503777431347</v>
       </c>
@@ -12059,12 +12059,12 @@
         <f>IFERROR(AVERAGE(G14:H14),"")</f>
         <v>42.875</v>
       </c>
-      <c r="J14" s="182">
+      <c r="J14" s="184">
         <f>(I14+I15)/(2*I14)</f>
         <v>1.0002915451895045</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A15" s="16">
         <v>300</v>
       </c>
@@ -12078,7 +12078,7 @@
         <f>IFERROR(AVERAGE(B15:C15),"")</f>
         <v>42.875</v>
       </c>
-      <c r="E15" s="182"/>
+      <c r="E15" s="184"/>
       <c r="F15" s="16">
         <v>300</v>
       </c>
@@ -12092,25 +12092,25 @@
         <f>IFERROR(AVERAGE(G15:H15),"")</f>
         <v>42.9</v>
       </c>
-      <c r="J15" s="182"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="183" t="s">
+      <c r="J15" s="184"/>
+    </row>
+    <row r="16" spans="1:16" ht="15" x14ac:dyDescent="0.45">
+      <c r="A16" s="182" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="184"/>
-      <c r="C16" s="184"/>
-      <c r="D16" s="184"/>
-      <c r="E16" s="186"/>
-      <c r="F16" s="183" t="s">
+      <c r="B16" s="183"/>
+      <c r="C16" s="183"/>
+      <c r="D16" s="183"/>
+      <c r="E16" s="185"/>
+      <c r="F16" s="182" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="184"/>
-      <c r="H16" s="184"/>
-      <c r="I16" s="184"/>
-      <c r="J16" s="184"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G16" s="183"/>
+      <c r="H16" s="183"/>
+      <c r="I16" s="183"/>
+      <c r="J16" s="183"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" s="14" t="s">
         <v>5</v>
       </c>
@@ -12138,7 +12138,7 @@
       </c>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A18" s="14">
         <v>150</v>
       </c>
@@ -12152,7 +12152,7 @@
         <f>IFERROR(AVERAGE(B18:C18),"")</f>
         <v>42.58</v>
       </c>
-      <c r="E18" s="182">
+      <c r="E18" s="184">
         <f>(1-A19/A18)/(D19/D18-A19/A18)</f>
         <v>1.0147759771210676</v>
       </c>
@@ -12169,12 +12169,12 @@
         <f>IFERROR(AVERAGE(G18:H18),"")</f>
         <v>43.2</v>
       </c>
-      <c r="J18" s="182">
+      <c r="J18" s="184">
         <f>(I18+I19)/(2*I18)</f>
         <v>1.0005208333333333</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A19" s="16">
         <v>300</v>
       </c>
@@ -12188,7 +12188,7 @@
         <f>IFERROR(AVERAGE(B19:C19),"")</f>
         <v>43.2</v>
       </c>
-      <c r="E19" s="182"/>
+      <c r="E19" s="184"/>
       <c r="F19" s="16">
         <v>300</v>
       </c>
@@ -12202,25 +12202,25 @@
         <f>IFERROR(AVERAGE(G19:H19),"")</f>
         <v>43.245000000000005</v>
       </c>
-      <c r="J19" s="182"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="183" t="s">
+      <c r="J19" s="184"/>
+    </row>
+    <row r="20" spans="1:10" ht="15" x14ac:dyDescent="0.45">
+      <c r="A20" s="182" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="184"/>
-      <c r="C20" s="184"/>
-      <c r="D20" s="184"/>
-      <c r="E20" s="186"/>
-      <c r="F20" s="183" t="s">
+      <c r="B20" s="183"/>
+      <c r="C20" s="183"/>
+      <c r="D20" s="183"/>
+      <c r="E20" s="185"/>
+      <c r="F20" s="182" t="s">
         <v>11</v>
       </c>
-      <c r="G20" s="184"/>
-      <c r="H20" s="184"/>
-      <c r="I20" s="184"/>
-      <c r="J20" s="184"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G20" s="183"/>
+      <c r="H20" s="183"/>
+      <c r="I20" s="183"/>
+      <c r="J20" s="183"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A21" s="14" t="s">
         <v>5</v>
       </c>
@@ -12248,7 +12248,7 @@
       </c>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A22" s="14">
         <v>150</v>
       </c>
@@ -12262,7 +12262,7 @@
         <f>IFERROR(AVERAGE(B22:C22),"")</f>
         <v>41.05</v>
       </c>
-      <c r="E22" s="182">
+      <c r="E22" s="184">
         <f>(1-A23/A22)/(D23/D22-A23/A22)</f>
         <v>1.0140810276679844</v>
       </c>
@@ -12279,12 +12279,12 @@
         <f>IFERROR(AVERAGE(G22:H22),"")</f>
         <v>41.620000000000005</v>
       </c>
-      <c r="J22" s="182">
+      <c r="J22" s="184">
         <f>(I22+I23)/(2*I22)</f>
         <v>1.000600672753484</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A23" s="16">
         <v>300</v>
       </c>
@@ -12298,7 +12298,7 @@
         <f>IFERROR(AVERAGE(B23:C23),"")</f>
         <v>41.620000000000005</v>
       </c>
-      <c r="E23" s="182"/>
+      <c r="E23" s="184"/>
       <c r="F23" s="16">
         <v>300</v>
       </c>
@@ -12312,25 +12312,25 @@
         <f>IFERROR(AVERAGE(G23:H23),"")</f>
         <v>41.67</v>
       </c>
-      <c r="J23" s="182"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="183" t="s">
+      <c r="J23" s="184"/>
+    </row>
+    <row r="24" spans="1:10" ht="15" x14ac:dyDescent="0.45">
+      <c r="A24" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="184"/>
-      <c r="C24" s="184"/>
-      <c r="D24" s="184"/>
-      <c r="E24" s="186"/>
-      <c r="F24" s="183" t="s">
+      <c r="B24" s="183"/>
+      <c r="C24" s="183"/>
+      <c r="D24" s="183"/>
+      <c r="E24" s="185"/>
+      <c r="F24" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="G24" s="184"/>
-      <c r="H24" s="184"/>
-      <c r="I24" s="184"/>
-      <c r="J24" s="184"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G24" s="183"/>
+      <c r="H24" s="183"/>
+      <c r="I24" s="183"/>
+      <c r="J24" s="183"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A25" s="14" t="s">
         <v>5</v>
       </c>
@@ -12358,7 +12358,7 @@
       </c>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A26" s="14">
         <v>150</v>
       </c>
@@ -12372,7 +12372,7 @@
         <f>IFERROR(AVERAGE(B26:C26),"")</f>
         <v>40.034999999999997</v>
       </c>
-      <c r="E26" s="182">
+      <c r="E26" s="184">
         <f>(1-A27/A26)/(D27/D26-A27/A26)</f>
         <v>1.0135443037974685</v>
       </c>
@@ -12389,12 +12389,12 @@
         <f>IFERROR(AVERAGE(G26:H26),"")</f>
         <v>40.57</v>
       </c>
-      <c r="J26" s="182">
+      <c r="J26" s="184">
         <f>(I26+I27)/(2*I26)</f>
         <v>1.0012324377618931</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A27" s="16">
         <v>300</v>
       </c>
@@ -12408,7 +12408,7 @@
         <f>IFERROR(AVERAGE(B27:C27),"")</f>
         <v>40.57</v>
       </c>
-      <c r="E27" s="182"/>
+      <c r="E27" s="184"/>
       <c r="F27" s="16">
         <v>300</v>
       </c>
@@ -12422,17 +12422,17 @@
         <f>IFERROR(AVERAGE(G27:H27),"")</f>
         <v>40.67</v>
       </c>
-      <c r="J27" s="182"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="185" t="s">
+      <c r="J27" s="184"/>
+    </row>
+    <row r="28" spans="1:10" ht="15" x14ac:dyDescent="0.45">
+      <c r="A28" s="189" t="s">
         <v>13</v>
       </c>
       <c r="B28" s="133"/>
       <c r="C28" s="133"/>
       <c r="D28" s="133"/>
-      <c r="E28" s="190"/>
-      <c r="F28" s="185" t="s">
+      <c r="E28" s="192"/>
+      <c r="F28" s="189" t="s">
         <v>13</v>
       </c>
       <c r="G28" s="133"/>
@@ -12440,7 +12440,7 @@
       <c r="I28" s="133"/>
       <c r="J28" s="133"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A29" s="14" t="s">
         <v>5</v>
       </c>
@@ -12468,7 +12468,7 @@
       </c>
       <c r="J29" s="5"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A30" s="14">
         <v>150</v>
       </c>
@@ -12482,7 +12482,7 @@
         <f>IFERROR(AVERAGE(B30:C30),"")</f>
         <v>39.105000000000004</v>
       </c>
-      <c r="E30" s="182">
+      <c r="E30" s="184">
         <f>(1-A31/A30)/(D31/D30-A31/A30)</f>
         <v>1.0132141469102212</v>
       </c>
@@ -12499,12 +12499,12 @@
         <f>IFERROR(AVERAGE(G30:H30),"")</f>
         <v>39.614999999999995</v>
       </c>
-      <c r="J30" s="182">
+      <c r="J30" s="184">
         <f>(I30+I31)/(2*I30)</f>
         <v>1.0003786444528588</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A31" s="16">
         <v>300</v>
       </c>
@@ -12518,7 +12518,7 @@
         <f>IFERROR(AVERAGE(B31:C31),"")</f>
         <v>39.614999999999995</v>
       </c>
-      <c r="E31" s="182"/>
+      <c r="E31" s="184"/>
       <c r="F31" s="16">
         <v>300</v>
       </c>
@@ -12532,63 +12532,46 @@
         <f>IFERROR(AVERAGE(G31:H31),"")</f>
         <v>39.644999999999996</v>
       </c>
-      <c r="J31" s="182"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="192"/>
-      <c r="B32" s="192"/>
-      <c r="C32" s="192"/>
-      <c r="D32" s="192"/>
-      <c r="E32" s="192"/>
-      <c r="F32" s="192"/>
-      <c r="G32" s="192"/>
-      <c r="H32" s="192"/>
-      <c r="I32" s="192"/>
-      <c r="J32" s="192"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" s="193"/>
-      <c r="B33" s="193"/>
-      <c r="C33" s="193"/>
-      <c r="D33" s="193"/>
-      <c r="E33" s="193"/>
-      <c r="F33" s="193"/>
-      <c r="G33" s="193"/>
-      <c r="H33" s="193"/>
-      <c r="I33" s="193"/>
-      <c r="J33" s="193"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="193"/>
-      <c r="B34" s="193"/>
-      <c r="C34" s="193"/>
-      <c r="D34" s="193"/>
-      <c r="E34" s="193"/>
-      <c r="F34" s="193"/>
-      <c r="G34" s="193"/>
-      <c r="H34" s="193"/>
-      <c r="I34" s="193"/>
-      <c r="J34" s="193"/>
+      <c r="J31" s="184"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A32" s="190"/>
+      <c r="B32" s="190"/>
+      <c r="C32" s="190"/>
+      <c r="D32" s="190"/>
+      <c r="E32" s="190"/>
+      <c r="F32" s="190"/>
+      <c r="G32" s="190"/>
+      <c r="H32" s="190"/>
+      <c r="I32" s="190"/>
+      <c r="J32" s="190"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A33" s="191"/>
+      <c r="B33" s="191"/>
+      <c r="C33" s="191"/>
+      <c r="D33" s="191"/>
+      <c r="E33" s="191"/>
+      <c r="F33" s="191"/>
+      <c r="G33" s="191"/>
+      <c r="H33" s="191"/>
+      <c r="I33" s="191"/>
+      <c r="J33" s="191"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A34" s="191"/>
+      <c r="B34" s="191"/>
+      <c r="C34" s="191"/>
+      <c r="D34" s="191"/>
+      <c r="E34" s="191"/>
+      <c r="F34" s="191"/>
+      <c r="G34" s="191"/>
+      <c r="H34" s="191"/>
+      <c r="I34" s="191"/>
+      <c r="J34" s="191"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="F20:J20"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="F3:J3"/>
-    <mergeCell ref="F4:J4"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="F8:J8"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="F12:J12"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="F16:J16"/>
-    <mergeCell ref="J30:J31"/>
-    <mergeCell ref="A32:J34"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="A28:E28"/>
     <mergeCell ref="J22:J23"/>
     <mergeCell ref="F24:J24"/>
     <mergeCell ref="J26:J27"/>
@@ -12605,6 +12588,23 @@
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A12:E12"/>
     <mergeCell ref="E14:E15"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="A32:J34"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="F20:J20"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="F4:J4"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="F8:J8"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="F12:J12"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="F16:J16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -12627,9 +12627,9 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>676275</xdr:colOff>
+                    <xdr:colOff>677333</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>219075</xdr:rowOff>
+                    <xdr:rowOff>220133</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -12649,7 +12649,7 @@
                   </from>
                   <to>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>962025</xdr:colOff>
+                    <xdr:colOff>960967</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -12667,13 +12667,13 @@
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>30</xdr:row>
-                    <xdr:rowOff>200025</xdr:rowOff>
+                    <xdr:rowOff>198967</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>971550</xdr:colOff>
+                    <xdr:colOff>973667</xdr:colOff>
                     <xdr:row>34</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
+                    <xdr:rowOff>173567</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -12697,31 +12697,31 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="26.625" customWidth="1"/>
-    <col min="2" max="2" width="22.75" customWidth="1"/>
-    <col min="3" max="3" width="12.375" customWidth="1"/>
+    <col min="1" max="1" width="26.609375" customWidth="1"/>
+    <col min="2" max="2" width="22.71875" customWidth="1"/>
+    <col min="3" max="3" width="12.38671875" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="29.5" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
-    <col min="7" max="7" width="20.375" customWidth="1"/>
-    <col min="8" max="8" width="26.375" customWidth="1"/>
-    <col min="15" max="15" width="11.625" customWidth="1"/>
+    <col min="7" max="7" width="20.38671875" customWidth="1"/>
+    <col min="8" max="8" width="26.38671875" customWidth="1"/>
+    <col min="15" max="15" width="11.609375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="203" t="s">
+    <row r="1" spans="1:15" ht="17" x14ac:dyDescent="0.4">
+      <c r="A1" s="204" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="203"/>
-      <c r="C1" s="203"/>
+      <c r="B1" s="204"/>
+      <c r="C1" s="204"/>
       <c r="O1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="200" t="s">
+    <row r="2" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="201" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="48" t="s">
@@ -12735,8 +12735,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="201"/>
+    <row r="3" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="202"/>
       <c r="B3" s="49" t="s">
         <v>37</v>
       </c>
@@ -12749,7 +12749,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="108"/>
       <c r="B4" s="12" t="s">
         <v>26</v>
@@ -12763,7 +12763,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="108"/>
       <c r="B5" s="13" t="s">
         <v>32</v>
@@ -12777,7 +12777,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="108"/>
       <c r="B6" s="32" t="s">
         <v>50</v>
@@ -12791,8 +12791,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="201" t="s">
+    <row r="7" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="202" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="50" t="str">
@@ -12808,8 +12808,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="201"/>
+    <row r="8" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="202"/>
       <c r="B8" s="34" t="str">
         <f>INDEX(MachineData,MATCH(SelectedMachine,Machines,0),4)&amp;"E"</f>
         <v>9E</v>
@@ -12823,8 +12823,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="201"/>
+    <row r="9" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="202"/>
       <c r="B9" s="34" t="str">
         <f>INDEX(MachineData,MATCH(SelectedMachine,Machines,0),5)&amp;"E"</f>
         <v>12E</v>
@@ -12838,8 +12838,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="201"/>
+    <row r="10" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="202"/>
       <c r="B10" s="34" t="str">
         <f>INDEX(MachineData,MATCH(SelectedMachine,Machines,0),6)&amp;"E"</f>
         <v>15E</v>
@@ -12853,8 +12853,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="202"/>
+    <row r="11" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="203"/>
       <c r="B11" s="49" t="str">
         <f>INDEX(MachineData,MATCH(SelectedMachine,Machines,0),7)&amp;"E"</f>
         <v>18E</v>
@@ -12868,7 +12868,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="109" t="s">
         <v>93</v>
       </c>
@@ -12882,53 +12882,53 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="204" t="s">
+    <row r="13" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="205" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="203"/>
-      <c r="C13" s="203"/>
+      <c r="B13" s="204"/>
+      <c r="C13" s="204"/>
       <c r="O13">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="110" t="s">
         <v>72</v>
       </c>
-      <c r="B14" s="205">
+      <c r="B14" s="206">
         <f>INDEX(ElectrometerFactors,MATCH(SelectedElectrometer,Electrometers,0),1)</f>
         <v>0.999</v>
       </c>
-      <c r="C14" s="206"/>
+      <c r="C14" s="207"/>
       <c r="O14">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="109" t="s">
         <v>93</v>
       </c>
-      <c r="B15" s="195">
+      <c r="B15" s="196">
         <f>INDEX(ElectrometerADCLDates,MATCH(SelectedElectrometer,Electrometers,0),1)</f>
         <v>42313</v>
       </c>
-      <c r="C15" s="196"/>
+      <c r="C15" s="197"/>
       <c r="O15">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="O16">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="176" t="s">
+    <row r="17" spans="1:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="164" t="s">
         <v>84</v>
       </c>
       <c r="B17" s="209" t="s">
@@ -12944,9 +12944,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="176"/>
-      <c r="B18" s="207" t="s">
+    <row r="18" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="164"/>
+      <c r="B18" s="208" t="s">
         <v>44</v>
       </c>
       <c r="C18" s="99" t="s">
@@ -12961,9 +12961,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="176"/>
-      <c r="B19" s="208"/>
+    <row r="19" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="164"/>
+      <c r="B19" s="195"/>
       <c r="C19" s="99" t="s">
         <v>37</v>
       </c>
@@ -12976,9 +12976,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="176"/>
-      <c r="B20" s="208"/>
+    <row r="20" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="164"/>
+      <c r="B20" s="195"/>
       <c r="C20" s="99" t="s">
         <v>39</v>
       </c>
@@ -12991,9 +12991,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="176"/>
-      <c r="B21" s="208"/>
+    <row r="21" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="164"/>
+      <c r="B21" s="195"/>
       <c r="C21" s="99" t="s">
         <v>40</v>
       </c>
@@ -13006,9 +13006,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="176"/>
-      <c r="B22" s="208"/>
+    <row r="22" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="164"/>
+      <c r="B22" s="195"/>
       <c r="C22" s="99" t="s">
         <v>41</v>
       </c>
@@ -13021,9 +13021,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="176"/>
-      <c r="B23" s="208"/>
+    <row r="23" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="164"/>
+      <c r="B23" s="195"/>
       <c r="C23" s="99" t="s">
         <v>42</v>
       </c>
@@ -13036,9 +13036,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="176"/>
-      <c r="B24" s="208"/>
+    <row r="24" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="164"/>
+      <c r="B24" s="195"/>
       <c r="C24" s="101" t="s">
         <v>43</v>
       </c>
@@ -13051,11 +13051,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="173" t="s">
+    <row r="25" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="180" t="s">
         <v>83</v>
       </c>
-      <c r="B25" s="208" t="s">
+      <c r="B25" s="195" t="s">
         <v>30</v>
       </c>
       <c r="C25" s="97" t="s">
@@ -13070,9 +13070,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="173"/>
-      <c r="B26" s="208"/>
+    <row r="26" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="180"/>
+      <c r="B26" s="195"/>
       <c r="C26" s="101" t="s">
         <v>37</v>
       </c>
@@ -13085,9 +13085,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="173"/>
-      <c r="B27" s="208" t="s">
+    <row r="27" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="180"/>
+      <c r="B27" s="195" t="s">
         <v>78</v>
       </c>
       <c r="C27" s="97" t="s">
@@ -13102,9 +13102,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="173"/>
-      <c r="B28" s="208"/>
+    <row r="28" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="180"/>
+      <c r="B28" s="195"/>
       <c r="C28" s="101" t="s">
         <v>37</v>
       </c>
@@ -13117,9 +13117,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="173"/>
-      <c r="B29" s="208" t="s">
+    <row r="29" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="180"/>
+      <c r="B29" s="195" t="s">
         <v>79</v>
       </c>
       <c r="C29" s="97" t="s">
@@ -13134,9 +13134,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="173"/>
-      <c r="B30" s="208"/>
+    <row r="30" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="180"/>
+      <c r="B30" s="195"/>
       <c r="C30" s="101" t="s">
         <v>37</v>
       </c>
@@ -13149,8 +13149,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="173"/>
+    <row r="31" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="180"/>
       <c r="B31" s="96" t="s">
         <v>45</v>
       </c>
@@ -13166,9 +13166,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="173"/>
-      <c r="B32" s="208" t="s">
+    <row r="32" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="180"/>
+      <c r="B32" s="195" t="s">
         <v>56</v>
       </c>
       <c r="C32" s="97" t="s">
@@ -13183,9 +13183,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="173"/>
-      <c r="B33" s="208"/>
+    <row r="33" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="180"/>
+      <c r="B33" s="195"/>
       <c r="C33" s="101" t="s">
         <v>37</v>
       </c>
@@ -13198,11 +13198,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="178" t="s">
+    <row r="34" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="166" t="s">
         <v>85</v>
       </c>
-      <c r="B34" s="208" t="s">
+      <c r="B34" s="195" t="s">
         <v>48</v>
       </c>
       <c r="C34" s="97" t="s">
@@ -13217,9 +13217,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="178"/>
-      <c r="B35" s="208"/>
+    <row r="35" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="166"/>
+      <c r="B35" s="195"/>
       <c r="C35" s="99" t="s">
         <v>40</v>
       </c>
@@ -13232,9 +13232,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="178"/>
-      <c r="B36" s="208"/>
+    <row r="36" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="166"/>
+      <c r="B36" s="195"/>
       <c r="C36" s="99" t="s">
         <v>41</v>
       </c>
@@ -13247,9 +13247,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="178"/>
-      <c r="B37" s="208"/>
+    <row r="37" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="166"/>
+      <c r="B37" s="195"/>
       <c r="C37" s="99" t="s">
         <v>42</v>
       </c>
@@ -13262,9 +13262,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="178"/>
-      <c r="B38" s="208"/>
+    <row r="38" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="166"/>
+      <c r="B38" s="195"/>
       <c r="C38" s="101" t="s">
         <v>43</v>
       </c>
@@ -13277,9 +13277,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="178"/>
-      <c r="B39" s="208" t="s">
+    <row r="39" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="166"/>
+      <c r="B39" s="195" t="s">
         <v>15</v>
       </c>
       <c r="C39" s="97" t="s">
@@ -13294,9 +13294,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="178"/>
-      <c r="B40" s="208"/>
+    <row r="40" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="166"/>
+      <c r="B40" s="195"/>
       <c r="C40" s="99" t="s">
         <v>40</v>
       </c>
@@ -13309,9 +13309,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="178"/>
-      <c r="B41" s="208"/>
+    <row r="41" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="166"/>
+      <c r="B41" s="195"/>
       <c r="C41" s="99" t="s">
         <v>41</v>
       </c>
@@ -13324,9 +13324,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="178"/>
-      <c r="B42" s="208"/>
+    <row r="42" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="166"/>
+      <c r="B42" s="195"/>
       <c r="C42" s="99" t="s">
         <v>42</v>
       </c>
@@ -13339,9 +13339,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="178"/>
-      <c r="B43" s="208"/>
+    <row r="43" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="166"/>
+      <c r="B43" s="195"/>
       <c r="C43" s="101" t="s">
         <v>43</v>
       </c>
@@ -13354,9 +13354,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="178"/>
-      <c r="B44" s="208" t="s">
+    <row r="44" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="166"/>
+      <c r="B44" s="195" t="s">
         <v>47</v>
       </c>
       <c r="C44" s="97" t="s">
@@ -13371,9 +13371,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="178"/>
-      <c r="B45" s="208"/>
+    <row r="45" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="166"/>
+      <c r="B45" s="195"/>
       <c r="C45" s="99" t="s">
         <v>40</v>
       </c>
@@ -13386,9 +13386,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="178"/>
-      <c r="B46" s="208"/>
+    <row r="46" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="166"/>
+      <c r="B46" s="195"/>
       <c r="C46" s="99" t="s">
         <v>41</v>
       </c>
@@ -13401,9 +13401,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="178"/>
-      <c r="B47" s="208"/>
+    <row r="47" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="166"/>
+      <c r="B47" s="195"/>
       <c r="C47" s="99" t="s">
         <v>42</v>
       </c>
@@ -13416,9 +13416,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="178"/>
-      <c r="B48" s="208"/>
+    <row r="48" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="166"/>
+      <c r="B48" s="195"/>
       <c r="C48" s="101" t="s">
         <v>43</v>
       </c>
@@ -13431,9 +13431,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="178"/>
-      <c r="B49" s="208" t="s">
+    <row r="49" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="166"/>
+      <c r="B49" s="195" t="s">
         <v>80</v>
       </c>
       <c r="C49" s="97" t="s">
@@ -13448,9 +13448,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="178"/>
-      <c r="B50" s="208"/>
+    <row r="50" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="166"/>
+      <c r="B50" s="195"/>
       <c r="C50" s="99" t="s">
         <v>40</v>
       </c>
@@ -13463,9 +13463,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="178"/>
-      <c r="B51" s="208"/>
+    <row r="51" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="166"/>
+      <c r="B51" s="195"/>
       <c r="C51" s="99" t="s">
         <v>41</v>
       </c>
@@ -13478,9 +13478,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="178"/>
-      <c r="B52" s="208"/>
+    <row r="52" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A52" s="166"/>
+      <c r="B52" s="195"/>
       <c r="C52" s="99" t="s">
         <v>42</v>
       </c>
@@ -13493,9 +13493,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="178"/>
-      <c r="B53" s="208"/>
+    <row r="53" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A53" s="166"/>
+      <c r="B53" s="195"/>
       <c r="C53" s="101" t="s">
         <v>43</v>
       </c>
@@ -13508,9 +13508,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="178"/>
-      <c r="B54" s="208" t="s">
+    <row r="54" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A54" s="166"/>
+      <c r="B54" s="195" t="s">
         <v>67</v>
       </c>
       <c r="C54" s="97" t="s">
@@ -13525,9 +13525,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="178"/>
-      <c r="B55" s="208"/>
+    <row r="55" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A55" s="166"/>
+      <c r="B55" s="195"/>
       <c r="C55" s="99" t="s">
         <v>40</v>
       </c>
@@ -13540,9 +13540,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="178"/>
-      <c r="B56" s="208"/>
+    <row r="56" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A56" s="166"/>
+      <c r="B56" s="195"/>
       <c r="C56" s="99" t="s">
         <v>41</v>
       </c>
@@ -13555,9 +13555,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A57" s="178"/>
-      <c r="B57" s="208"/>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A57" s="166"/>
+      <c r="B57" s="195"/>
       <c r="C57" s="99" t="s">
         <v>42</v>
       </c>
@@ -13570,9 +13570,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A58" s="178"/>
-      <c r="B58" s="208"/>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A58" s="166"/>
+      <c r="B58" s="195"/>
       <c r="C58" s="101" t="s">
         <v>43</v>
       </c>
@@ -13585,9 +13585,9 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A59" s="178"/>
-      <c r="B59" s="208" t="s">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A59" s="166"/>
+      <c r="B59" s="195" t="s">
         <v>81</v>
       </c>
       <c r="C59" s="97" t="s">
@@ -13602,9 +13602,9 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A60" s="178"/>
-      <c r="B60" s="208"/>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A60" s="166"/>
+      <c r="B60" s="195"/>
       <c r="C60" s="99" t="s">
         <v>40</v>
       </c>
@@ -13617,9 +13617,9 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A61" s="178"/>
-      <c r="B61" s="208"/>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A61" s="166"/>
+      <c r="B61" s="195"/>
       <c r="C61" s="99" t="s">
         <v>41</v>
       </c>
@@ -13632,9 +13632,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A62" s="178"/>
-      <c r="B62" s="208"/>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A62" s="166"/>
+      <c r="B62" s="195"/>
       <c r="C62" s="99" t="s">
         <v>42</v>
       </c>
@@ -13647,9 +13647,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A63" s="178"/>
-      <c r="B63" s="208"/>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A63" s="166"/>
+      <c r="B63" s="195"/>
       <c r="C63" s="101" t="s">
         <v>43</v>
       </c>
@@ -13662,9 +13662,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A64" s="178"/>
-      <c r="B64" s="208" t="s">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A64" s="166"/>
+      <c r="B64" s="195" t="s">
         <v>87</v>
       </c>
       <c r="C64" s="97" t="s">
@@ -13679,9 +13679,9 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A65" s="178"/>
-      <c r="B65" s="208"/>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A65" s="166"/>
+      <c r="B65" s="195"/>
       <c r="C65" s="99" t="s">
         <v>40</v>
       </c>
@@ -13694,9 +13694,9 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A66" s="178"/>
-      <c r="B66" s="208"/>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A66" s="166"/>
+      <c r="B66" s="195"/>
       <c r="C66" s="105" t="s">
         <v>41</v>
       </c>
@@ -13709,9 +13709,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A67" s="178"/>
-      <c r="B67" s="208"/>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A67" s="166"/>
+      <c r="B67" s="195"/>
       <c r="C67" s="99" t="s">
         <v>42</v>
       </c>
@@ -13724,9 +13724,9 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A68" s="178"/>
-      <c r="B68" s="208"/>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A68" s="166"/>
+      <c r="B68" s="195"/>
       <c r="C68" s="101" t="s">
         <v>43</v>
       </c>
@@ -13739,9 +13739,9 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A69" s="178"/>
-      <c r="B69" s="208" t="s">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A69" s="166"/>
+      <c r="B69" s="195" t="s">
         <v>88</v>
       </c>
       <c r="C69" s="97" t="s">
@@ -13756,9 +13756,9 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A70" s="178"/>
-      <c r="B70" s="208"/>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A70" s="166"/>
+      <c r="B70" s="195"/>
       <c r="C70" s="99" t="s">
         <v>40</v>
       </c>
@@ -13771,9 +13771,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A71" s="178"/>
-      <c r="B71" s="208"/>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A71" s="166"/>
+      <c r="B71" s="195"/>
       <c r="C71" s="105" t="s">
         <v>41</v>
       </c>
@@ -13786,9 +13786,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A72" s="178"/>
-      <c r="B72" s="208"/>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A72" s="166"/>
+      <c r="B72" s="195"/>
       <c r="C72" s="99" t="s">
         <v>42</v>
       </c>
@@ -13801,9 +13801,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A73" s="178"/>
-      <c r="B73" s="208"/>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A73" s="166"/>
+      <c r="B73" s="195"/>
       <c r="C73" s="101" t="s">
         <v>43</v>
       </c>
@@ -13816,11 +13816,11 @@
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A74" s="180" t="s">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A74" s="168" t="s">
         <v>86</v>
       </c>
-      <c r="B74" s="208" t="s">
+      <c r="B74" s="195" t="s">
         <v>77</v>
       </c>
       <c r="C74" s="97" t="s">
@@ -13835,9 +13835,9 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A75" s="181"/>
-      <c r="B75" s="208"/>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A75" s="169"/>
+      <c r="B75" s="195"/>
       <c r="C75" s="99" t="s">
         <v>40</v>
       </c>
@@ -13850,9 +13850,9 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A76" s="181"/>
-      <c r="B76" s="208"/>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A76" s="169"/>
+      <c r="B76" s="195"/>
       <c r="C76" s="99" t="s">
         <v>41</v>
       </c>
@@ -13865,9 +13865,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A77" s="181"/>
-      <c r="B77" s="208"/>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A77" s="169"/>
+      <c r="B77" s="195"/>
       <c r="C77" s="99" t="s">
         <v>42</v>
       </c>
@@ -13876,9 +13876,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A78" s="181"/>
-      <c r="B78" s="208"/>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A78" s="169"/>
+      <c r="B78" s="195"/>
       <c r="C78" s="101" t="s">
         <v>43</v>
       </c>
@@ -13887,9 +13887,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A79" s="181"/>
-      <c r="B79" s="208" t="s">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A79" s="169"/>
+      <c r="B79" s="195" t="s">
         <v>4</v>
       </c>
       <c r="C79" s="97" t="s">
@@ -13900,9 +13900,9 @@
         <v>1.0038684719535782</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A80" s="181"/>
-      <c r="B80" s="208"/>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A80" s="169"/>
+      <c r="B80" s="195"/>
       <c r="C80" s="99" t="s">
         <v>37</v>
       </c>
@@ -13911,9 +13911,9 @@
         <v>1.0058199246833277</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" s="181"/>
-      <c r="B81" s="208"/>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A81" s="169"/>
+      <c r="B81" s="195"/>
       <c r="C81" s="99" t="s">
         <v>39</v>
       </c>
@@ -13922,9 +13922,9 @@
         <v>1.0149903288201161</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" s="181"/>
-      <c r="B82" s="208"/>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A82" s="169"/>
+      <c r="B82" s="195"/>
       <c r="C82" s="106" t="s">
         <v>40</v>
       </c>
@@ -13933,9 +13933,9 @@
         <v>1.0137799952482776</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" s="181"/>
-      <c r="B83" s="208"/>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A83" s="169"/>
+      <c r="B83" s="195"/>
       <c r="C83" s="99" t="s">
         <v>41</v>
       </c>
@@ -13944,9 +13944,9 @@
         <v>1.011832946635731</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="181"/>
-      <c r="B84" s="208"/>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A84" s="169"/>
+      <c r="B84" s="195"/>
       <c r="C84" s="106" t="s">
         <v>42</v>
       </c>
@@ -13955,9 +13955,9 @@
         <v>1.0128956623681125</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" s="181"/>
-      <c r="B85" s="208"/>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A85" s="169"/>
+      <c r="B85" s="195"/>
       <c r="C85" s="101" t="s">
         <v>43</v>
       </c>
@@ -13966,9 +13966,9 @@
         <v>1.0151151631477926</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" s="181"/>
-      <c r="B86" s="208" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A86" s="169"/>
+      <c r="B86" s="195" t="s">
         <v>14</v>
       </c>
       <c r="C86" s="97" t="s">
@@ -13979,9 +13979,9 @@
         <v>0.99980806142034551</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" s="181"/>
-      <c r="B87" s="208"/>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A87" s="169"/>
+      <c r="B87" s="195"/>
       <c r="C87" s="99" t="s">
         <v>37</v>
       </c>
@@ -13990,9 +13990,9 @@
         <v>0.99966159052453474</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" s="181"/>
-      <c r="B88" s="208"/>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A88" s="169"/>
+      <c r="B88" s="195"/>
       <c r="C88" s="99" t="s">
         <v>39</v>
       </c>
@@ -14001,9 +14001,9 @@
         <v>1.0009389671361502</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" s="181"/>
-      <c r="B89" s="208"/>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A89" s="169"/>
+      <c r="B89" s="195"/>
       <c r="C89" s="99" t="s">
         <v>40</v>
       </c>
@@ -14012,9 +14012,9 @@
         <v>1.0002312138728324</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" s="181"/>
-      <c r="B90" s="208"/>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A90" s="169"/>
+      <c r="B90" s="195"/>
       <c r="C90" s="99" t="s">
         <v>41</v>
       </c>
@@ -14023,9 +14023,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" s="181"/>
-      <c r="B91" s="208"/>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A91" s="169"/>
+      <c r="B91" s="195"/>
       <c r="C91" s="99" t="s">
         <v>42</v>
       </c>
@@ -14034,9 +14034,9 @@
         <v>1.0003428571428572</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A92" s="181"/>
-      <c r="B92" s="208"/>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A92" s="169"/>
+      <c r="B92" s="195"/>
       <c r="C92" s="101" t="s">
         <v>43</v>
       </c>
@@ -14045,12 +14045,12 @@
         <v>1.0006986492780625</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93" s="197" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A93" s="198" t="s">
         <v>62</v>
       </c>
-      <c r="B93" s="198"/>
-      <c r="C93" s="199"/>
+      <c r="B93" s="199"/>
+      <c r="C93" s="200"/>
       <c r="D93" s="107" t="b">
         <f>INDEX(MachineData,MATCH(SelectedMachine,Machines,0),76)</f>
         <v>1</v>
@@ -14058,18 +14058,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A34:A73"/>
-    <mergeCell ref="B49:B53"/>
-    <mergeCell ref="B54:B58"/>
-    <mergeCell ref="B59:B63"/>
-    <mergeCell ref="B64:B68"/>
-    <mergeCell ref="B69:B73"/>
-    <mergeCell ref="B74:B78"/>
-    <mergeCell ref="B79:B85"/>
-    <mergeCell ref="B86:B92"/>
-    <mergeCell ref="B34:B38"/>
-    <mergeCell ref="B39:B43"/>
-    <mergeCell ref="B44:B48"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="A93:C93"/>
     <mergeCell ref="A2:A3"/>
@@ -14086,6 +14074,18 @@
     <mergeCell ref="B32:B33"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="A74:A92"/>
+    <mergeCell ref="B74:B78"/>
+    <mergeCell ref="B79:B85"/>
+    <mergeCell ref="B86:B92"/>
+    <mergeCell ref="B34:B38"/>
+    <mergeCell ref="B39:B43"/>
+    <mergeCell ref="B44:B48"/>
+    <mergeCell ref="A34:A73"/>
+    <mergeCell ref="B49:B53"/>
+    <mergeCell ref="B54:B58"/>
+    <mergeCell ref="B59:B63"/>
+    <mergeCell ref="B64:B68"/>
+    <mergeCell ref="B69:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="4"/>
@@ -17515,7 +17515,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D8B6EA4-CFA4-4FC6-BFED-A13CC201B88D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{704F3662-0AC8-45FE-A41F-18DF799A656C}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
@@ -17527,7 +17527,7 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{704F3662-0AC8-45FE-A41F-18DF799A656C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D8B6EA4-CFA4-4FC6-BFED-A13CC201B88D}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>

</xml_diff>